<commit_message>
Updated for September 2015 release
</commit_message>
<xml_diff>
--- a/DTAPI/Doc/CapList.xlsx
+++ b/DTAPI/Doc/CapList.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="354">
   <si>
     <t>Group</t>
   </si>
@@ -653,6 +653,9 @@
     <t>TX_ATSC</t>
   </si>
   <si>
+    <t>TX_ATSC3</t>
+  </si>
+  <si>
     <t>TX_CMMB</t>
   </si>
   <si>
@@ -876,6 +879,9 @@
   </si>
   <si>
     <t>ATSC 8-VSB modulation</t>
+  </si>
+  <si>
+    <t>ATSC3.0 modulation</t>
   </si>
   <si>
     <t>CMMB modulation</t>
@@ -17279,7 +17285,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CM126"/>
+  <dimension ref="A1:CM127"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
@@ -17302,7 +17308,7 @@
     <row r="1" spans="1:91" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="93"/>
       <c r="B1" s="95" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="C1" s="93"/>
       <c r="D1" s="93"/>
@@ -17770,7 +17776,7 @@
         <v>93</v>
       </c>
       <c r="BF3" s="77" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="BG3" s="66">
         <v>8</v>
@@ -17788,7 +17794,7 @@
         <v>93</v>
       </c>
       <c r="BL3" s="77" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="BM3" s="66">
         <v>8</v>
@@ -17967,7 +17973,7 @@
         <v>183</v>
       </c>
       <c r="CL4" s="84" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="CM4" s="93"/>
     </row>
@@ -18165,7 +18171,7 @@
         <v>185</v>
       </c>
       <c r="CL6" s="88" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="CM6" s="93"/>
     </row>
@@ -18266,7 +18272,7 @@
         <v>187</v>
       </c>
       <c r="CL7" s="89" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="CM7" s="93"/>
     </row>
@@ -18365,7 +18371,7 @@
         <v>188</v>
       </c>
       <c r="CL8" s="25" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="CM8" s="93"/>
     </row>
@@ -18464,7 +18470,7 @@
         <v>189</v>
       </c>
       <c r="CL9" s="92" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="CM9" s="93"/>
     </row>
@@ -18567,7 +18573,7 @@
         <v>191</v>
       </c>
       <c r="CL10" s="84" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="CM10" s="93"/>
     </row>
@@ -18666,7 +18672,7 @@
         <v>192</v>
       </c>
       <c r="CL11" s="86" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="CM11" s="93"/>
     </row>
@@ -18787,7 +18793,7 @@
         <v>193</v>
       </c>
       <c r="CL12" s="86" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="CM12" s="93"/>
     </row>
@@ -18886,7 +18892,7 @@
         <v>194</v>
       </c>
       <c r="CL13" s="86" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="CM13" s="93"/>
     </row>
@@ -18993,7 +18999,7 @@
         <v>195</v>
       </c>
       <c r="CL14" s="86" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="CM14" s="93"/>
     </row>
@@ -19092,7 +19098,7 @@
         <v>196</v>
       </c>
       <c r="CL15" s="86" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="CM15" s="93"/>
     </row>
@@ -19197,7 +19203,7 @@
         <v>197</v>
       </c>
       <c r="CL16" s="86" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="CM16" s="93"/>
     </row>
@@ -19308,7 +19314,7 @@
         <v>198</v>
       </c>
       <c r="CL17" s="86" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="CM17" s="93"/>
     </row>
@@ -19411,7 +19417,7 @@
         <v>199</v>
       </c>
       <c r="CL18" s="86" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="CM18" s="93"/>
     </row>
@@ -19518,7 +19524,7 @@
         <v>200</v>
       </c>
       <c r="CL19" s="86" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="CM19" s="93"/>
     </row>
@@ -19621,7 +19627,7 @@
         <v>201</v>
       </c>
       <c r="CL20" s="86" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="CM20" s="93"/>
     </row>
@@ -19752,7 +19758,7 @@
         <v>202</v>
       </c>
       <c r="CL21" s="86" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="CM21" s="93"/>
     </row>
@@ -19853,7 +19859,7 @@
         <v>203</v>
       </c>
       <c r="CL22" s="86" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="CM22" s="93"/>
     </row>
@@ -19970,7 +19976,7 @@
         <v>204</v>
       </c>
       <c r="CL23" s="86" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="CM23" s="93"/>
     </row>
@@ -20069,7 +20075,7 @@
         <v>205</v>
       </c>
       <c r="CL24" s="88" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="CM24" s="93"/>
     </row>
@@ -20170,7 +20176,7 @@
         <v>207</v>
       </c>
       <c r="CL25" s="89" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="CM25" s="93"/>
     </row>
@@ -20189,15 +20195,15 @@
       <c r="J26" s="40"/>
       <c r="K26" s="40"/>
       <c r="L26" s="40"/>
-      <c r="M26" s="98"/>
+      <c r="M26" s="40"/>
       <c r="N26" s="38"/>
-      <c r="O26" s="104"/>
+      <c r="O26" s="58"/>
       <c r="P26" s="38"/>
-      <c r="Q26" s="104"/>
+      <c r="Q26" s="58"/>
       <c r="R26" s="38"/>
-      <c r="S26" s="104"/>
+      <c r="S26" s="58"/>
       <c r="T26" s="38"/>
-      <c r="U26" s="104"/>
+      <c r="U26" s="58"/>
       <c r="V26" s="40"/>
       <c r="W26" s="40"/>
       <c r="X26" s="40"/>
@@ -20208,7 +20214,7 @@
       <c r="AC26" s="38"/>
       <c r="AD26" s="58"/>
       <c r="AE26" s="40"/>
-      <c r="AF26" s="98"/>
+      <c r="AF26" s="40"/>
       <c r="AG26" s="98"/>
       <c r="AH26" s="40"/>
       <c r="AI26" s="38"/>
@@ -20247,7 +20253,7 @@
       <c r="BP26" s="56"/>
       <c r="BQ26" s="58"/>
       <c r="BR26" s="40"/>
-      <c r="BS26" s="98"/>
+      <c r="BS26" s="40"/>
       <c r="BT26" s="40"/>
       <c r="BU26" s="40"/>
       <c r="BV26" s="40"/>
@@ -20269,7 +20275,7 @@
         <v>208</v>
       </c>
       <c r="CL26" s="25" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="CM26" s="93"/>
     </row>
@@ -20306,7 +20312,7 @@
       <c r="AB27" s="58"/>
       <c r="AC27" s="38"/>
       <c r="AD27" s="58"/>
-      <c r="AE27" s="98"/>
+      <c r="AE27" s="40"/>
       <c r="AF27" s="98"/>
       <c r="AG27" s="98"/>
       <c r="AH27" s="40"/>
@@ -20368,7 +20374,7 @@
         <v>209</v>
       </c>
       <c r="CL27" s="25" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="CM27" s="93"/>
     </row>
@@ -20405,7 +20411,7 @@
       <c r="AB28" s="58"/>
       <c r="AC28" s="38"/>
       <c r="AD28" s="58"/>
-      <c r="AE28" s="40"/>
+      <c r="AE28" s="98"/>
       <c r="AF28" s="98"/>
       <c r="AG28" s="98"/>
       <c r="AH28" s="40"/>
@@ -20467,7 +20473,7 @@
         <v>210</v>
       </c>
       <c r="CL28" s="25" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="CM28" s="93"/>
     </row>
@@ -20566,7 +20572,7 @@
         <v>211</v>
       </c>
       <c r="CL29" s="25" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="CM29" s="93"/>
     </row>
@@ -20583,17 +20589,17 @@
       <c r="H30" s="40"/>
       <c r="I30" s="40"/>
       <c r="J30" s="40"/>
-      <c r="K30" s="42"/>
+      <c r="K30" s="40"/>
       <c r="L30" s="40"/>
-      <c r="M30" s="40"/>
+      <c r="M30" s="98"/>
       <c r="N30" s="38"/>
-      <c r="O30" s="58"/>
+      <c r="O30" s="104"/>
       <c r="P30" s="38"/>
-      <c r="Q30" s="58"/>
+      <c r="Q30" s="104"/>
       <c r="R30" s="38"/>
-      <c r="S30" s="58"/>
+      <c r="S30" s="104"/>
       <c r="T30" s="38"/>
-      <c r="U30" s="58"/>
+      <c r="U30" s="104"/>
       <c r="V30" s="40"/>
       <c r="W30" s="40"/>
       <c r="X30" s="40"/>
@@ -20603,9 +20609,9 @@
       <c r="AB30" s="58"/>
       <c r="AC30" s="38"/>
       <c r="AD30" s="58"/>
-      <c r="AE30" s="42"/>
-      <c r="AF30" s="40"/>
-      <c r="AG30" s="42"/>
+      <c r="AE30" s="40"/>
+      <c r="AF30" s="98"/>
+      <c r="AG30" s="98"/>
       <c r="AH30" s="40"/>
       <c r="AI30" s="38"/>
       <c r="AJ30" s="58"/>
@@ -20643,7 +20649,7 @@
       <c r="BP30" s="56"/>
       <c r="BQ30" s="58"/>
       <c r="BR30" s="40"/>
-      <c r="BS30" s="40"/>
+      <c r="BS30" s="98"/>
       <c r="BT30" s="40"/>
       <c r="BU30" s="40"/>
       <c r="BV30" s="40"/>
@@ -20655,17 +20661,17 @@
       <c r="CB30" s="58"/>
       <c r="CC30" s="38"/>
       <c r="CD30" s="58"/>
-      <c r="CE30" s="42"/>
-      <c r="CF30" s="42"/>
-      <c r="CG30" s="42"/>
-      <c r="CH30" s="42"/>
+      <c r="CE30" s="98"/>
+      <c r="CF30" s="98"/>
+      <c r="CG30" s="98"/>
+      <c r="CH30" s="98"/>
       <c r="CI30" s="40"/>
       <c r="CJ30" s="40"/>
       <c r="CK30" s="90" t="s">
         <v>212</v>
       </c>
       <c r="CL30" s="25" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="CM30" s="93"/>
     </row>
@@ -20682,7 +20688,7 @@
       <c r="H31" s="40"/>
       <c r="I31" s="40"/>
       <c r="J31" s="40"/>
-      <c r="K31" s="98"/>
+      <c r="K31" s="42"/>
       <c r="L31" s="40"/>
       <c r="M31" s="40"/>
       <c r="N31" s="38"/>
@@ -20764,7 +20770,7 @@
         <v>213</v>
       </c>
       <c r="CL31" s="25" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="CM31" s="93"/>
     </row>
@@ -20781,7 +20787,7 @@
       <c r="H32" s="40"/>
       <c r="I32" s="40"/>
       <c r="J32" s="40"/>
-      <c r="K32" s="40"/>
+      <c r="K32" s="98"/>
       <c r="L32" s="40"/>
       <c r="M32" s="40"/>
       <c r="N32" s="38"/>
@@ -20801,9 +20807,9 @@
       <c r="AB32" s="58"/>
       <c r="AC32" s="38"/>
       <c r="AD32" s="58"/>
-      <c r="AE32" s="40"/>
+      <c r="AE32" s="42"/>
       <c r="AF32" s="40"/>
-      <c r="AG32" s="98"/>
+      <c r="AG32" s="42"/>
       <c r="AH32" s="40"/>
       <c r="AI32" s="38"/>
       <c r="AJ32" s="58"/>
@@ -20853,17 +20859,17 @@
       <c r="CB32" s="58"/>
       <c r="CC32" s="38"/>
       <c r="CD32" s="58"/>
-      <c r="CE32" s="98"/>
-      <c r="CF32" s="98"/>
-      <c r="CG32" s="98"/>
-      <c r="CH32" s="98"/>
+      <c r="CE32" s="42"/>
+      <c r="CF32" s="42"/>
+      <c r="CG32" s="42"/>
+      <c r="CH32" s="42"/>
       <c r="CI32" s="40"/>
       <c r="CJ32" s="40"/>
       <c r="CK32" s="90" t="s">
         <v>214</v>
       </c>
       <c r="CL32" s="25" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="CM32" s="93"/>
     </row>
@@ -20882,15 +20888,15 @@
       <c r="J33" s="40"/>
       <c r="K33" s="40"/>
       <c r="L33" s="40"/>
-      <c r="M33" s="42"/>
+      <c r="M33" s="40"/>
       <c r="N33" s="38"/>
-      <c r="O33" s="62"/>
+      <c r="O33" s="58"/>
       <c r="P33" s="38"/>
-      <c r="Q33" s="62"/>
+      <c r="Q33" s="58"/>
       <c r="R33" s="38"/>
-      <c r="S33" s="62"/>
+      <c r="S33" s="58"/>
       <c r="T33" s="38"/>
-      <c r="U33" s="62"/>
+      <c r="U33" s="58"/>
       <c r="V33" s="40"/>
       <c r="W33" s="40"/>
       <c r="X33" s="40"/>
@@ -20900,9 +20906,9 @@
       <c r="AB33" s="58"/>
       <c r="AC33" s="38"/>
       <c r="AD33" s="58"/>
-      <c r="AE33" s="42"/>
-      <c r="AF33" s="42"/>
-      <c r="AG33" s="42"/>
+      <c r="AE33" s="40"/>
+      <c r="AF33" s="40"/>
+      <c r="AG33" s="98"/>
       <c r="AH33" s="40"/>
       <c r="AI33" s="38"/>
       <c r="AJ33" s="58"/>
@@ -20940,7 +20946,7 @@
       <c r="BP33" s="56"/>
       <c r="BQ33" s="58"/>
       <c r="BR33" s="40"/>
-      <c r="BS33" s="42"/>
+      <c r="BS33" s="40"/>
       <c r="BT33" s="40"/>
       <c r="BU33" s="40"/>
       <c r="BV33" s="40"/>
@@ -20952,17 +20958,17 @@
       <c r="CB33" s="58"/>
       <c r="CC33" s="38"/>
       <c r="CD33" s="58"/>
-      <c r="CE33" s="42"/>
-      <c r="CF33" s="42"/>
-      <c r="CG33" s="42"/>
-      <c r="CH33" s="42"/>
+      <c r="CE33" s="98"/>
+      <c r="CF33" s="98"/>
+      <c r="CG33" s="98"/>
+      <c r="CH33" s="98"/>
       <c r="CI33" s="40"/>
       <c r="CJ33" s="40"/>
       <c r="CK33" s="90" t="s">
         <v>215</v>
       </c>
       <c r="CL33" s="25" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="CM33" s="93"/>
     </row>
@@ -20981,15 +20987,15 @@
       <c r="J34" s="40"/>
       <c r="K34" s="40"/>
       <c r="L34" s="40"/>
-      <c r="M34" s="98"/>
+      <c r="M34" s="42"/>
       <c r="N34" s="38"/>
-      <c r="O34" s="104"/>
+      <c r="O34" s="62"/>
       <c r="P34" s="38"/>
-      <c r="Q34" s="104"/>
+      <c r="Q34" s="62"/>
       <c r="R34" s="38"/>
-      <c r="S34" s="104"/>
+      <c r="S34" s="62"/>
       <c r="T34" s="38"/>
-      <c r="U34" s="104"/>
+      <c r="U34" s="62"/>
       <c r="V34" s="40"/>
       <c r="W34" s="40"/>
       <c r="X34" s="40"/>
@@ -20999,9 +21005,9 @@
       <c r="AB34" s="58"/>
       <c r="AC34" s="38"/>
       <c r="AD34" s="58"/>
-      <c r="AE34" s="98"/>
-      <c r="AF34" s="98"/>
-      <c r="AG34" s="98"/>
+      <c r="AE34" s="42"/>
+      <c r="AF34" s="42"/>
+      <c r="AG34" s="42"/>
       <c r="AH34" s="40"/>
       <c r="AI34" s="38"/>
       <c r="AJ34" s="58"/>
@@ -21039,7 +21045,7 @@
       <c r="BP34" s="56"/>
       <c r="BQ34" s="58"/>
       <c r="BR34" s="40"/>
-      <c r="BS34" s="98"/>
+      <c r="BS34" s="42"/>
       <c r="BT34" s="40"/>
       <c r="BU34" s="40"/>
       <c r="BV34" s="40"/>
@@ -21051,17 +21057,17 @@
       <c r="CB34" s="58"/>
       <c r="CC34" s="38"/>
       <c r="CD34" s="58"/>
-      <c r="CE34" s="98"/>
-      <c r="CF34" s="98"/>
-      <c r="CG34" s="98"/>
-      <c r="CH34" s="98"/>
+      <c r="CE34" s="42"/>
+      <c r="CF34" s="42"/>
+      <c r="CG34" s="42"/>
+      <c r="CH34" s="42"/>
       <c r="CI34" s="40"/>
       <c r="CJ34" s="40"/>
       <c r="CK34" s="90" t="s">
         <v>216</v>
       </c>
       <c r="CL34" s="25" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="CM34" s="93"/>
     </row>
@@ -21082,13 +21088,13 @@
       <c r="L35" s="40"/>
       <c r="M35" s="98"/>
       <c r="N35" s="38"/>
-      <c r="O35" s="58"/>
+      <c r="O35" s="104"/>
       <c r="P35" s="38"/>
       <c r="Q35" s="104"/>
       <c r="R35" s="38"/>
-      <c r="S35" s="58"/>
+      <c r="S35" s="104"/>
       <c r="T35" s="38"/>
-      <c r="U35" s="58"/>
+      <c r="U35" s="104"/>
       <c r="V35" s="40"/>
       <c r="W35" s="40"/>
       <c r="X35" s="40"/>
@@ -21098,7 +21104,7 @@
       <c r="AB35" s="58"/>
       <c r="AC35" s="38"/>
       <c r="AD35" s="58"/>
-      <c r="AE35" s="40"/>
+      <c r="AE35" s="98"/>
       <c r="AF35" s="98"/>
       <c r="AG35" s="98"/>
       <c r="AH35" s="40"/>
@@ -21160,7 +21166,7 @@
         <v>217</v>
       </c>
       <c r="CL35" s="25" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="CM35" s="93"/>
     </row>
@@ -21181,13 +21187,13 @@
       <c r="L36" s="40"/>
       <c r="M36" s="98"/>
       <c r="N36" s="38"/>
-      <c r="O36" s="104"/>
+      <c r="O36" s="58"/>
       <c r="P36" s="38"/>
       <c r="Q36" s="104"/>
       <c r="R36" s="38"/>
-      <c r="S36" s="104"/>
+      <c r="S36" s="58"/>
       <c r="T36" s="38"/>
-      <c r="U36" s="104"/>
+      <c r="U36" s="58"/>
       <c r="V36" s="40"/>
       <c r="W36" s="40"/>
       <c r="X36" s="40"/>
@@ -21197,7 +21203,7 @@
       <c r="AB36" s="58"/>
       <c r="AC36" s="38"/>
       <c r="AD36" s="58"/>
-      <c r="AE36" s="98"/>
+      <c r="AE36" s="40"/>
       <c r="AF36" s="98"/>
       <c r="AG36" s="98"/>
       <c r="AH36" s="40"/>
@@ -21259,7 +21265,7 @@
         <v>218</v>
       </c>
       <c r="CL36" s="25" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="CM36" s="93"/>
     </row>
@@ -21276,17 +21282,17 @@
       <c r="H37" s="40"/>
       <c r="I37" s="40"/>
       <c r="J37" s="40"/>
-      <c r="K37" s="98"/>
+      <c r="K37" s="40"/>
       <c r="L37" s="40"/>
-      <c r="M37" s="40"/>
+      <c r="M37" s="98"/>
       <c r="N37" s="38"/>
-      <c r="O37" s="58"/>
+      <c r="O37" s="104"/>
       <c r="P37" s="38"/>
-      <c r="Q37" s="58"/>
+      <c r="Q37" s="104"/>
       <c r="R37" s="38"/>
-      <c r="S37" s="58"/>
+      <c r="S37" s="104"/>
       <c r="T37" s="38"/>
-      <c r="U37" s="58"/>
+      <c r="U37" s="104"/>
       <c r="V37" s="40"/>
       <c r="W37" s="40"/>
       <c r="X37" s="40"/>
@@ -21297,7 +21303,7 @@
       <c r="AC37" s="38"/>
       <c r="AD37" s="58"/>
       <c r="AE37" s="98"/>
-      <c r="AF37" s="40"/>
+      <c r="AF37" s="98"/>
       <c r="AG37" s="98"/>
       <c r="AH37" s="40"/>
       <c r="AI37" s="38"/>
@@ -21336,7 +21342,7 @@
       <c r="BP37" s="56"/>
       <c r="BQ37" s="58"/>
       <c r="BR37" s="40"/>
-      <c r="BS37" s="40"/>
+      <c r="BS37" s="98"/>
       <c r="BT37" s="40"/>
       <c r="BU37" s="40"/>
       <c r="BV37" s="40"/>
@@ -21358,7 +21364,7 @@
         <v>219</v>
       </c>
       <c r="CL37" s="25" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="CM37" s="93"/>
     </row>
@@ -21375,17 +21381,17 @@
       <c r="H38" s="40"/>
       <c r="I38" s="40"/>
       <c r="J38" s="40"/>
-      <c r="K38" s="40"/>
+      <c r="K38" s="98"/>
       <c r="L38" s="40"/>
-      <c r="M38" s="98"/>
+      <c r="M38" s="40"/>
       <c r="N38" s="38"/>
-      <c r="O38" s="104"/>
+      <c r="O38" s="58"/>
       <c r="P38" s="38"/>
-      <c r="Q38" s="104"/>
+      <c r="Q38" s="58"/>
       <c r="R38" s="38"/>
-      <c r="S38" s="104"/>
+      <c r="S38" s="58"/>
       <c r="T38" s="38"/>
-      <c r="U38" s="104"/>
+      <c r="U38" s="58"/>
       <c r="V38" s="40"/>
       <c r="W38" s="40"/>
       <c r="X38" s="40"/>
@@ -21396,7 +21402,7 @@
       <c r="AC38" s="38"/>
       <c r="AD38" s="58"/>
       <c r="AE38" s="98"/>
-      <c r="AF38" s="98"/>
+      <c r="AF38" s="40"/>
       <c r="AG38" s="98"/>
       <c r="AH38" s="40"/>
       <c r="AI38" s="38"/>
@@ -21435,7 +21441,7 @@
       <c r="BP38" s="56"/>
       <c r="BQ38" s="58"/>
       <c r="BR38" s="40"/>
-      <c r="BS38" s="98"/>
+      <c r="BS38" s="40"/>
       <c r="BT38" s="40"/>
       <c r="BU38" s="40"/>
       <c r="BV38" s="40"/>
@@ -21457,7 +21463,7 @@
         <v>220</v>
       </c>
       <c r="CL38" s="25" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="CM38" s="93"/>
     </row>
@@ -21556,7 +21562,7 @@
         <v>221</v>
       </c>
       <c r="CL39" s="25" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="CM39" s="93"/>
     </row>
@@ -21593,7 +21599,7 @@
       <c r="AB40" s="58"/>
       <c r="AC40" s="38"/>
       <c r="AD40" s="58"/>
-      <c r="AE40" s="40"/>
+      <c r="AE40" s="98"/>
       <c r="AF40" s="98"/>
       <c r="AG40" s="98"/>
       <c r="AH40" s="40"/>
@@ -21655,7 +21661,7 @@
         <v>222</v>
       </c>
       <c r="CL40" s="25" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="CM40" s="93"/>
     </row>
@@ -21673,16 +21679,16 @@
       <c r="I41" s="40"/>
       <c r="J41" s="40"/>
       <c r="K41" s="40"/>
-      <c r="L41" s="42"/>
-      <c r="M41" s="42"/>
+      <c r="L41" s="40"/>
+      <c r="M41" s="98"/>
       <c r="N41" s="38"/>
-      <c r="O41" s="62"/>
+      <c r="O41" s="104"/>
       <c r="P41" s="38"/>
-      <c r="Q41" s="62"/>
+      <c r="Q41" s="104"/>
       <c r="R41" s="38"/>
-      <c r="S41" s="62"/>
+      <c r="S41" s="104"/>
       <c r="T41" s="38"/>
-      <c r="U41" s="62"/>
+      <c r="U41" s="104"/>
       <c r="V41" s="40"/>
       <c r="W41" s="40"/>
       <c r="X41" s="40"/>
@@ -21693,8 +21699,8 @@
       <c r="AC41" s="38"/>
       <c r="AD41" s="58"/>
       <c r="AE41" s="40"/>
-      <c r="AF41" s="42"/>
-      <c r="AG41" s="42"/>
+      <c r="AF41" s="98"/>
+      <c r="AG41" s="98"/>
       <c r="AH41" s="40"/>
       <c r="AI41" s="38"/>
       <c r="AJ41" s="58"/>
@@ -21732,7 +21738,7 @@
       <c r="BP41" s="56"/>
       <c r="BQ41" s="58"/>
       <c r="BR41" s="40"/>
-      <c r="BS41" s="42"/>
+      <c r="BS41" s="98"/>
       <c r="BT41" s="40"/>
       <c r="BU41" s="40"/>
       <c r="BV41" s="40"/>
@@ -21744,17 +21750,17 @@
       <c r="CB41" s="58"/>
       <c r="CC41" s="38"/>
       <c r="CD41" s="58"/>
-      <c r="CE41" s="42"/>
-      <c r="CF41" s="42"/>
-      <c r="CG41" s="42"/>
-      <c r="CH41" s="42"/>
+      <c r="CE41" s="98"/>
+      <c r="CF41" s="98"/>
+      <c r="CG41" s="98"/>
+      <c r="CH41" s="98"/>
       <c r="CI41" s="40"/>
       <c r="CJ41" s="40"/>
       <c r="CK41" s="90" t="s">
         <v>223</v>
       </c>
       <c r="CL41" s="25" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="CM41" s="93"/>
     </row>
@@ -21772,14 +21778,12 @@
       <c r="I42" s="40"/>
       <c r="J42" s="40"/>
       <c r="K42" s="40"/>
-      <c r="L42" s="40"/>
+      <c r="L42" s="42"/>
       <c r="M42" s="42"/>
       <c r="N42" s="38"/>
       <c r="O42" s="62"/>
       <c r="P42" s="38"/>
-      <c r="Q42" s="71">
-        <v>1</v>
-      </c>
+      <c r="Q42" s="62"/>
       <c r="R42" s="38"/>
       <c r="S42" s="62"/>
       <c r="T42" s="38"/>
@@ -21855,7 +21859,7 @@
         <v>224</v>
       </c>
       <c r="CL42" s="25" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="CM42" s="93"/>
     </row>
@@ -21873,12 +21877,14 @@
       <c r="I43" s="40"/>
       <c r="J43" s="40"/>
       <c r="K43" s="40"/>
-      <c r="L43" s="42"/>
+      <c r="L43" s="40"/>
       <c r="M43" s="42"/>
       <c r="N43" s="38"/>
       <c r="O43" s="62"/>
       <c r="P43" s="38"/>
-      <c r="Q43" s="62"/>
+      <c r="Q43" s="71">
+        <v>1</v>
+      </c>
       <c r="R43" s="38"/>
       <c r="S43" s="62"/>
       <c r="T43" s="38"/>
@@ -21954,7 +21960,7 @@
         <v>225</v>
       </c>
       <c r="CL43" s="25" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="CM43" s="93"/>
     </row>
@@ -21972,16 +21978,16 @@
       <c r="I44" s="40"/>
       <c r="J44" s="40"/>
       <c r="K44" s="40"/>
-      <c r="L44" s="40"/>
-      <c r="M44" s="40"/>
+      <c r="L44" s="42"/>
+      <c r="M44" s="42"/>
       <c r="N44" s="38"/>
-      <c r="O44" s="58"/>
+      <c r="O44" s="62"/>
       <c r="P44" s="38"/>
-      <c r="Q44" s="58"/>
+      <c r="Q44" s="62"/>
       <c r="R44" s="38"/>
-      <c r="S44" s="58"/>
+      <c r="S44" s="62"/>
       <c r="T44" s="38"/>
-      <c r="U44" s="58"/>
+      <c r="U44" s="62"/>
       <c r="V44" s="40"/>
       <c r="W44" s="40"/>
       <c r="X44" s="40"/>
@@ -21992,8 +21998,8 @@
       <c r="AC44" s="38"/>
       <c r="AD44" s="58"/>
       <c r="AE44" s="40"/>
-      <c r="AF44" s="98"/>
-      <c r="AG44" s="98"/>
+      <c r="AF44" s="42"/>
+      <c r="AG44" s="42"/>
       <c r="AH44" s="40"/>
       <c r="AI44" s="38"/>
       <c r="AJ44" s="58"/>
@@ -22031,7 +22037,7 @@
       <c r="BP44" s="56"/>
       <c r="BQ44" s="58"/>
       <c r="BR44" s="40"/>
-      <c r="BS44" s="40"/>
+      <c r="BS44" s="42"/>
       <c r="BT44" s="40"/>
       <c r="BU44" s="40"/>
       <c r="BV44" s="40"/>
@@ -22043,17 +22049,17 @@
       <c r="CB44" s="58"/>
       <c r="CC44" s="38"/>
       <c r="CD44" s="58"/>
-      <c r="CE44" s="40"/>
-      <c r="CF44" s="40"/>
-      <c r="CG44" s="40"/>
-      <c r="CH44" s="40"/>
+      <c r="CE44" s="42"/>
+      <c r="CF44" s="42"/>
+      <c r="CG44" s="42"/>
+      <c r="CH44" s="42"/>
       <c r="CI44" s="40"/>
       <c r="CJ44" s="40"/>
       <c r="CK44" s="90" t="s">
         <v>226</v>
       </c>
       <c r="CL44" s="25" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="CM44" s="93"/>
     </row>
@@ -22067,71 +22073,69 @@
       <c r="E45" s="40"/>
       <c r="F45" s="40"/>
       <c r="G45" s="40"/>
-      <c r="H45" s="98"/>
+      <c r="H45" s="40"/>
       <c r="I45" s="40"/>
-      <c r="J45" s="98"/>
+      <c r="J45" s="40"/>
       <c r="K45" s="40"/>
       <c r="L45" s="40"/>
       <c r="M45" s="40"/>
-      <c r="N45" s="103"/>
+      <c r="N45" s="38"/>
       <c r="O45" s="58"/>
-      <c r="P45" s="103"/>
+      <c r="P45" s="38"/>
       <c r="Q45" s="58"/>
-      <c r="R45" s="103"/>
+      <c r="R45" s="38"/>
       <c r="S45" s="58"/>
-      <c r="T45" s="103"/>
+      <c r="T45" s="38"/>
       <c r="U45" s="58"/>
       <c r="V45" s="40"/>
       <c r="W45" s="40"/>
       <c r="X45" s="40"/>
       <c r="Y45" s="38"/>
-      <c r="Z45" s="104"/>
-      <c r="AA45" s="103"/>
-      <c r="AB45" s="104"/>
-      <c r="AC45" s="103"/>
-      <c r="AD45" s="104"/>
+      <c r="Z45" s="58"/>
+      <c r="AA45" s="38"/>
+      <c r="AB45" s="58"/>
+      <c r="AC45" s="38"/>
+      <c r="AD45" s="58"/>
       <c r="AE45" s="40"/>
-      <c r="AF45" s="40"/>
-      <c r="AG45" s="40"/>
+      <c r="AF45" s="98"/>
+      <c r="AG45" s="98"/>
       <c r="AH45" s="40"/>
       <c r="AI45" s="38"/>
       <c r="AJ45" s="58"/>
       <c r="AK45" s="38"/>
-      <c r="AL45" s="104"/>
+      <c r="AL45" s="58"/>
       <c r="AM45" s="38"/>
       <c r="AN45" s="56"/>
-      <c r="AO45" s="104"/>
+      <c r="AO45" s="58"/>
       <c r="AP45" s="38"/>
       <c r="AQ45" s="56"/>
-      <c r="AR45" s="104"/>
+      <c r="AR45" s="58"/>
       <c r="AS45" s="40"/>
       <c r="AT45" s="40"/>
       <c r="AU45" s="40"/>
       <c r="AV45" s="38"/>
       <c r="AW45" s="58"/>
-      <c r="AX45" s="98"/>
-      <c r="AY45" s="98"/>
-      <c r="AZ45" s="103"/>
-      <c r="BA45" s="104"/>
-      <c r="BB45" s="107">
-        <v>2</v>
-      </c>
+      <c r="AX45" s="40"/>
+      <c r="AY45" s="40"/>
+      <c r="AZ45" s="38"/>
+      <c r="BA45" s="58"/>
+      <c r="BB45" s="38"/>
       <c r="BC45" s="56"/>
       <c r="BD45" s="58"/>
-      <c r="BE45" s="103"/>
+      <c r="BE45" s="38"/>
       <c r="BF45" s="56"/>
       <c r="BG45" s="58"/>
-      <c r="BH45" s="103"/>
-      <c r="BI45" s="104"/>
-      <c r="BJ45" s="98"/>
-      <c r="BK45" s="103"/>
+      <c r="BH45" s="38"/>
+      <c r="BI45" s="58"/>
+      <c r="BJ45" s="40"/>
+      <c r="BK45" s="38"/>
       <c r="BL45" s="56"/>
       <c r="BM45" s="58"/>
-      <c r="BN45" s="103"/>
+      <c r="BN45" s="38"/>
       <c r="BO45" s="56"/>
       <c r="BP45" s="56"/>
       <c r="BQ45" s="58"/>
-      <c r="BR45" s="98"/>
+      <c r="BR45" s="40"/>
       <c r="BS45" s="40"/>
       <c r="BT45" s="40"/>
       <c r="BU45" s="40"/>
@@ -22143,7 +22147,7 @@
       <c r="CA45" s="38"/>
       <c r="CB45" s="58"/>
       <c r="CC45" s="38"/>
-      <c r="CD45" s="104"/>
+      <c r="CD45" s="58"/>
       <c r="CE45" s="40"/>
       <c r="CF45" s="40"/>
       <c r="CG45" s="40"/>
@@ -22154,308 +22158,310 @@
         <v>227</v>
       </c>
       <c r="CL45" s="25" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="CM45" s="93"/>
     </row>
-    <row r="46" spans="1:91" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A46" s="93"/>
-      <c r="B46" s="31"/>
-      <c r="C46" s="92" t="s">
+      <c r="B46" s="30"/>
+      <c r="C46" s="25" t="s">
         <v>228</v>
       </c>
-      <c r="D46" s="41"/>
-      <c r="E46" s="41"/>
-      <c r="F46" s="41"/>
-      <c r="G46" s="41"/>
-      <c r="H46" s="41"/>
-      <c r="I46" s="41"/>
-      <c r="J46" s="41"/>
-      <c r="K46" s="41"/>
-      <c r="L46" s="41"/>
-      <c r="M46" s="102"/>
-      <c r="N46" s="59"/>
-      <c r="O46" s="105"/>
-      <c r="P46" s="59"/>
-      <c r="Q46" s="105"/>
-      <c r="R46" s="59"/>
-      <c r="S46" s="105"/>
-      <c r="T46" s="59"/>
-      <c r="U46" s="105"/>
-      <c r="V46" s="41"/>
-      <c r="W46" s="41"/>
-      <c r="X46" s="41"/>
-      <c r="Y46" s="59"/>
-      <c r="Z46" s="60"/>
-      <c r="AA46" s="59"/>
-      <c r="AB46" s="60"/>
-      <c r="AC46" s="59"/>
-      <c r="AD46" s="60"/>
-      <c r="AE46" s="41"/>
-      <c r="AF46" s="102"/>
-      <c r="AG46" s="67"/>
-      <c r="AH46" s="41"/>
-      <c r="AI46" s="59"/>
-      <c r="AJ46" s="60"/>
-      <c r="AK46" s="59"/>
-      <c r="AL46" s="60"/>
-      <c r="AM46" s="59"/>
-      <c r="AN46" s="74"/>
-      <c r="AO46" s="60"/>
-      <c r="AP46" s="59"/>
-      <c r="AQ46" s="74"/>
-      <c r="AR46" s="60"/>
-      <c r="AS46" s="41"/>
-      <c r="AT46" s="41"/>
-      <c r="AU46" s="41"/>
-      <c r="AV46" s="59"/>
-      <c r="AW46" s="60"/>
-      <c r="AX46" s="41"/>
-      <c r="AY46" s="41"/>
-      <c r="AZ46" s="59"/>
-      <c r="BA46" s="60"/>
-      <c r="BB46" s="59"/>
-      <c r="BC46" s="74"/>
-      <c r="BD46" s="60"/>
-      <c r="BE46" s="59"/>
-      <c r="BF46" s="74"/>
-      <c r="BG46" s="60"/>
-      <c r="BH46" s="59"/>
-      <c r="BI46" s="60"/>
-      <c r="BJ46" s="41"/>
-      <c r="BK46" s="59"/>
-      <c r="BL46" s="74"/>
-      <c r="BM46" s="60"/>
-      <c r="BN46" s="59"/>
-      <c r="BO46" s="74"/>
-      <c r="BP46" s="74"/>
-      <c r="BQ46" s="60"/>
-      <c r="BR46" s="41"/>
-      <c r="BS46" s="102"/>
-      <c r="BT46" s="41"/>
-      <c r="BU46" s="41"/>
-      <c r="BV46" s="41"/>
-      <c r="BW46" s="59"/>
-      <c r="BX46" s="60"/>
-      <c r="BY46" s="59"/>
-      <c r="BZ46" s="60"/>
-      <c r="CA46" s="59"/>
-      <c r="CB46" s="60"/>
-      <c r="CC46" s="59"/>
-      <c r="CD46" s="60"/>
-      <c r="CE46" s="102"/>
-      <c r="CF46" s="102"/>
-      <c r="CG46" s="102"/>
-      <c r="CH46" s="102"/>
-      <c r="CI46" s="41"/>
-      <c r="CJ46" s="41"/>
-      <c r="CK46" s="91" t="s">
+      <c r="D46" s="40"/>
+      <c r="E46" s="40"/>
+      <c r="F46" s="40"/>
+      <c r="G46" s="40"/>
+      <c r="H46" s="98"/>
+      <c r="I46" s="40"/>
+      <c r="J46" s="98"/>
+      <c r="K46" s="40"/>
+      <c r="L46" s="40"/>
+      <c r="M46" s="40"/>
+      <c r="N46" s="103"/>
+      <c r="O46" s="58"/>
+      <c r="P46" s="103"/>
+      <c r="Q46" s="58"/>
+      <c r="R46" s="103"/>
+      <c r="S46" s="58"/>
+      <c r="T46" s="103"/>
+      <c r="U46" s="58"/>
+      <c r="V46" s="40"/>
+      <c r="W46" s="40"/>
+      <c r="X46" s="40"/>
+      <c r="Y46" s="38"/>
+      <c r="Z46" s="104"/>
+      <c r="AA46" s="103"/>
+      <c r="AB46" s="104"/>
+      <c r="AC46" s="103"/>
+      <c r="AD46" s="104"/>
+      <c r="AE46" s="40"/>
+      <c r="AF46" s="40"/>
+      <c r="AG46" s="40"/>
+      <c r="AH46" s="40"/>
+      <c r="AI46" s="38"/>
+      <c r="AJ46" s="58"/>
+      <c r="AK46" s="38"/>
+      <c r="AL46" s="104"/>
+      <c r="AM46" s="38"/>
+      <c r="AN46" s="56"/>
+      <c r="AO46" s="104"/>
+      <c r="AP46" s="38"/>
+      <c r="AQ46" s="56"/>
+      <c r="AR46" s="104"/>
+      <c r="AS46" s="40"/>
+      <c r="AT46" s="40"/>
+      <c r="AU46" s="40"/>
+      <c r="AV46" s="38"/>
+      <c r="AW46" s="58"/>
+      <c r="AX46" s="98"/>
+      <c r="AY46" s="98"/>
+      <c r="AZ46" s="103"/>
+      <c r="BA46" s="104"/>
+      <c r="BB46" s="107">
+        <v>2</v>
+      </c>
+      <c r="BC46" s="56"/>
+      <c r="BD46" s="58"/>
+      <c r="BE46" s="103"/>
+      <c r="BF46" s="56"/>
+      <c r="BG46" s="58"/>
+      <c r="BH46" s="103"/>
+      <c r="BI46" s="104"/>
+      <c r="BJ46" s="98"/>
+      <c r="BK46" s="103"/>
+      <c r="BL46" s="56"/>
+      <c r="BM46" s="58"/>
+      <c r="BN46" s="103"/>
+      <c r="BO46" s="56"/>
+      <c r="BP46" s="56"/>
+      <c r="BQ46" s="58"/>
+      <c r="BR46" s="98"/>
+      <c r="BS46" s="40"/>
+      <c r="BT46" s="40"/>
+      <c r="BU46" s="40"/>
+      <c r="BV46" s="40"/>
+      <c r="BW46" s="38"/>
+      <c r="BX46" s="58"/>
+      <c r="BY46" s="38"/>
+      <c r="BZ46" s="58"/>
+      <c r="CA46" s="38"/>
+      <c r="CB46" s="58"/>
+      <c r="CC46" s="38"/>
+      <c r="CD46" s="104"/>
+      <c r="CE46" s="40"/>
+      <c r="CF46" s="40"/>
+      <c r="CG46" s="40"/>
+      <c r="CH46" s="40"/>
+      <c r="CI46" s="40"/>
+      <c r="CJ46" s="40"/>
+      <c r="CK46" s="90" t="s">
         <v>228</v>
       </c>
-      <c r="CL46" s="92" t="s">
-        <v>303</v>
+      <c r="CL46" s="25" t="s">
+        <v>304</v>
       </c>
       <c r="CM46" s="93"/>
     </row>
-    <row r="47" spans="1:91" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:91" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="93"/>
-      <c r="B47" s="15" t="s">
+      <c r="B47" s="31"/>
+      <c r="C47" s="92" t="s">
         <v>229</v>
       </c>
-      <c r="C47" s="84" t="s">
-        <v>230</v>
-      </c>
-      <c r="D47" s="34"/>
-      <c r="E47" s="34"/>
-      <c r="F47" s="34"/>
-      <c r="G47" s="34"/>
-      <c r="H47" s="34"/>
-      <c r="I47" s="34"/>
-      <c r="J47" s="34"/>
-      <c r="K47" s="100">
-        <v>3</v>
-      </c>
-      <c r="L47" s="34"/>
-      <c r="M47" s="34"/>
-      <c r="N47" s="32"/>
-      <c r="O47" s="81"/>
-      <c r="P47" s="32"/>
-      <c r="Q47" s="81"/>
-      <c r="R47" s="32"/>
-      <c r="S47" s="51"/>
-      <c r="T47" s="32"/>
-      <c r="U47" s="51"/>
-      <c r="V47" s="34"/>
-      <c r="W47" s="34"/>
-      <c r="X47" s="34"/>
-      <c r="Y47" s="32"/>
-      <c r="Z47" s="51"/>
-      <c r="AA47" s="32"/>
-      <c r="AB47" s="51"/>
-      <c r="AC47" s="32"/>
-      <c r="AD47" s="51"/>
-      <c r="AE47" s="48"/>
-      <c r="AF47" s="48"/>
-      <c r="AG47" s="48"/>
-      <c r="AH47" s="34"/>
-      <c r="AI47" s="32"/>
-      <c r="AJ47" s="51"/>
-      <c r="AK47" s="32"/>
-      <c r="AL47" s="51"/>
-      <c r="AM47" s="32"/>
-      <c r="AN47" s="49"/>
-      <c r="AO47" s="51"/>
-      <c r="AP47" s="32"/>
-      <c r="AQ47" s="49"/>
-      <c r="AR47" s="51"/>
-      <c r="AS47" s="34"/>
-      <c r="AT47" s="34"/>
-      <c r="AU47" s="34"/>
-      <c r="AV47" s="32"/>
-      <c r="AW47" s="51"/>
-      <c r="AX47" s="34"/>
-      <c r="AY47" s="34"/>
-      <c r="AZ47" s="32"/>
-      <c r="BA47" s="51"/>
-      <c r="BB47" s="32"/>
-      <c r="BC47" s="49"/>
-      <c r="BD47" s="51"/>
-      <c r="BE47" s="32"/>
-      <c r="BF47" s="49"/>
-      <c r="BG47" s="51"/>
-      <c r="BH47" s="32"/>
-      <c r="BI47" s="51"/>
-      <c r="BJ47" s="34"/>
-      <c r="BK47" s="32"/>
-      <c r="BL47" s="49"/>
-      <c r="BM47" s="51"/>
-      <c r="BN47" s="32"/>
-      <c r="BO47" s="49"/>
-      <c r="BP47" s="49"/>
-      <c r="BQ47" s="51"/>
-      <c r="BR47" s="34"/>
-      <c r="BS47" s="48"/>
-      <c r="BT47" s="34"/>
-      <c r="BU47" s="34"/>
-      <c r="BV47" s="34"/>
-      <c r="BW47" s="32"/>
-      <c r="BX47" s="51"/>
-      <c r="BY47" s="32"/>
-      <c r="BZ47" s="51"/>
-      <c r="CA47" s="32"/>
-      <c r="CB47" s="51"/>
-      <c r="CC47" s="32"/>
-      <c r="CD47" s="51"/>
-      <c r="CE47" s="48"/>
-      <c r="CF47" s="48"/>
-      <c r="CG47" s="48"/>
-      <c r="CH47" s="48"/>
-      <c r="CI47" s="34"/>
-      <c r="CJ47" s="34"/>
-      <c r="CK47" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="CL47" s="84" t="s">
-        <v>304</v>
+      <c r="D47" s="41"/>
+      <c r="E47" s="41"/>
+      <c r="F47" s="41"/>
+      <c r="G47" s="41"/>
+      <c r="H47" s="41"/>
+      <c r="I47" s="41"/>
+      <c r="J47" s="41"/>
+      <c r="K47" s="41"/>
+      <c r="L47" s="41"/>
+      <c r="M47" s="102"/>
+      <c r="N47" s="59"/>
+      <c r="O47" s="105"/>
+      <c r="P47" s="59"/>
+      <c r="Q47" s="105"/>
+      <c r="R47" s="59"/>
+      <c r="S47" s="105"/>
+      <c r="T47" s="59"/>
+      <c r="U47" s="105"/>
+      <c r="V47" s="41"/>
+      <c r="W47" s="41"/>
+      <c r="X47" s="41"/>
+      <c r="Y47" s="59"/>
+      <c r="Z47" s="60"/>
+      <c r="AA47" s="59"/>
+      <c r="AB47" s="60"/>
+      <c r="AC47" s="59"/>
+      <c r="AD47" s="60"/>
+      <c r="AE47" s="41"/>
+      <c r="AF47" s="102"/>
+      <c r="AG47" s="67"/>
+      <c r="AH47" s="41"/>
+      <c r="AI47" s="59"/>
+      <c r="AJ47" s="60"/>
+      <c r="AK47" s="59"/>
+      <c r="AL47" s="60"/>
+      <c r="AM47" s="59"/>
+      <c r="AN47" s="74"/>
+      <c r="AO47" s="60"/>
+      <c r="AP47" s="59"/>
+      <c r="AQ47" s="74"/>
+      <c r="AR47" s="60"/>
+      <c r="AS47" s="41"/>
+      <c r="AT47" s="41"/>
+      <c r="AU47" s="41"/>
+      <c r="AV47" s="59"/>
+      <c r="AW47" s="60"/>
+      <c r="AX47" s="41"/>
+      <c r="AY47" s="41"/>
+      <c r="AZ47" s="59"/>
+      <c r="BA47" s="60"/>
+      <c r="BB47" s="59"/>
+      <c r="BC47" s="74"/>
+      <c r="BD47" s="60"/>
+      <c r="BE47" s="59"/>
+      <c r="BF47" s="74"/>
+      <c r="BG47" s="60"/>
+      <c r="BH47" s="59"/>
+      <c r="BI47" s="60"/>
+      <c r="BJ47" s="41"/>
+      <c r="BK47" s="59"/>
+      <c r="BL47" s="74"/>
+      <c r="BM47" s="60"/>
+      <c r="BN47" s="59"/>
+      <c r="BO47" s="74"/>
+      <c r="BP47" s="74"/>
+      <c r="BQ47" s="60"/>
+      <c r="BR47" s="41"/>
+      <c r="BS47" s="102"/>
+      <c r="BT47" s="41"/>
+      <c r="BU47" s="41"/>
+      <c r="BV47" s="41"/>
+      <c r="BW47" s="59"/>
+      <c r="BX47" s="60"/>
+      <c r="BY47" s="59"/>
+      <c r="BZ47" s="60"/>
+      <c r="CA47" s="59"/>
+      <c r="CB47" s="60"/>
+      <c r="CC47" s="59"/>
+      <c r="CD47" s="60"/>
+      <c r="CE47" s="67"/>
+      <c r="CF47" s="67"/>
+      <c r="CG47" s="67"/>
+      <c r="CH47" s="67"/>
+      <c r="CI47" s="41"/>
+      <c r="CJ47" s="41"/>
+      <c r="CK47" s="91" t="s">
+        <v>229</v>
+      </c>
+      <c r="CL47" s="92" t="s">
+        <v>305</v>
       </c>
       <c r="CM47" s="93"/>
     </row>
     <row r="48" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A48" s="93"/>
-      <c r="B48" s="16"/>
-      <c r="C48" s="86" t="s">
+      <c r="B48" s="15" t="s">
+        <v>230</v>
+      </c>
+      <c r="C48" s="84" t="s">
         <v>231</v>
       </c>
-      <c r="D48" s="35"/>
-      <c r="E48" s="35"/>
-      <c r="F48" s="35"/>
-      <c r="G48" s="35"/>
-      <c r="H48" s="35"/>
-      <c r="I48" s="35"/>
-      <c r="J48" s="35"/>
-      <c r="K48" s="35"/>
-      <c r="L48" s="35"/>
-      <c r="M48" s="98"/>
-      <c r="N48" s="33"/>
-      <c r="O48" s="104"/>
-      <c r="P48" s="33"/>
-      <c r="Q48" s="104"/>
-      <c r="R48" s="33"/>
-      <c r="S48" s="104"/>
-      <c r="T48" s="33"/>
-      <c r="U48" s="104"/>
-      <c r="V48" s="35"/>
-      <c r="W48" s="35"/>
-      <c r="X48" s="35"/>
-      <c r="Y48" s="33"/>
-      <c r="Z48" s="52"/>
-      <c r="AA48" s="33"/>
-      <c r="AB48" s="52"/>
-      <c r="AC48" s="33"/>
-      <c r="AD48" s="52"/>
-      <c r="AE48" s="98"/>
-      <c r="AF48" s="98"/>
-      <c r="AG48" s="98"/>
-      <c r="AH48" s="35"/>
-      <c r="AI48" s="33"/>
-      <c r="AJ48" s="52"/>
-      <c r="AK48" s="33"/>
-      <c r="AL48" s="52"/>
-      <c r="AM48" s="33"/>
-      <c r="AN48" s="50"/>
-      <c r="AO48" s="52"/>
-      <c r="AP48" s="33"/>
-      <c r="AQ48" s="50"/>
-      <c r="AR48" s="52"/>
-      <c r="AS48" s="35"/>
-      <c r="AT48" s="35"/>
-      <c r="AU48" s="35"/>
-      <c r="AV48" s="33"/>
-      <c r="AW48" s="52"/>
-      <c r="AX48" s="35"/>
-      <c r="AY48" s="35"/>
-      <c r="AZ48" s="33"/>
-      <c r="BA48" s="52"/>
-      <c r="BB48" s="33"/>
-      <c r="BC48" s="50"/>
-      <c r="BD48" s="52"/>
-      <c r="BE48" s="33"/>
-      <c r="BF48" s="50"/>
-      <c r="BG48" s="52"/>
-      <c r="BH48" s="33"/>
-      <c r="BI48" s="52"/>
-      <c r="BJ48" s="35"/>
-      <c r="BK48" s="33"/>
-      <c r="BL48" s="50"/>
-      <c r="BM48" s="52"/>
-      <c r="BN48" s="33"/>
-      <c r="BO48" s="50"/>
-      <c r="BP48" s="50"/>
-      <c r="BQ48" s="52"/>
-      <c r="BR48" s="35"/>
-      <c r="BS48" s="98"/>
-      <c r="BT48" s="35"/>
-      <c r="BU48" s="35"/>
-      <c r="BV48" s="35"/>
-      <c r="BW48" s="33"/>
-      <c r="BX48" s="52"/>
-      <c r="BY48" s="33"/>
-      <c r="BZ48" s="52"/>
-      <c r="CA48" s="33"/>
-      <c r="CB48" s="52"/>
-      <c r="CC48" s="33"/>
-      <c r="CD48" s="52"/>
-      <c r="CE48" s="98"/>
-      <c r="CF48" s="98"/>
-      <c r="CG48" s="98"/>
-      <c r="CH48" s="98"/>
-      <c r="CI48" s="35"/>
-      <c r="CJ48" s="35"/>
-      <c r="CK48" s="85" t="s">
+      <c r="D48" s="34"/>
+      <c r="E48" s="34"/>
+      <c r="F48" s="34"/>
+      <c r="G48" s="34"/>
+      <c r="H48" s="34"/>
+      <c r="I48" s="34"/>
+      <c r="J48" s="34"/>
+      <c r="K48" s="100">
+        <v>3</v>
+      </c>
+      <c r="L48" s="34"/>
+      <c r="M48" s="34"/>
+      <c r="N48" s="32"/>
+      <c r="O48" s="81"/>
+      <c r="P48" s="32"/>
+      <c r="Q48" s="81"/>
+      <c r="R48" s="32"/>
+      <c r="S48" s="51"/>
+      <c r="T48" s="32"/>
+      <c r="U48" s="51"/>
+      <c r="V48" s="34"/>
+      <c r="W48" s="34"/>
+      <c r="X48" s="34"/>
+      <c r="Y48" s="32"/>
+      <c r="Z48" s="51"/>
+      <c r="AA48" s="32"/>
+      <c r="AB48" s="51"/>
+      <c r="AC48" s="32"/>
+      <c r="AD48" s="51"/>
+      <c r="AE48" s="48"/>
+      <c r="AF48" s="48"/>
+      <c r="AG48" s="48"/>
+      <c r="AH48" s="34"/>
+      <c r="AI48" s="32"/>
+      <c r="AJ48" s="51"/>
+      <c r="AK48" s="32"/>
+      <c r="AL48" s="51"/>
+      <c r="AM48" s="32"/>
+      <c r="AN48" s="49"/>
+      <c r="AO48" s="51"/>
+      <c r="AP48" s="32"/>
+      <c r="AQ48" s="49"/>
+      <c r="AR48" s="51"/>
+      <c r="AS48" s="34"/>
+      <c r="AT48" s="34"/>
+      <c r="AU48" s="34"/>
+      <c r="AV48" s="32"/>
+      <c r="AW48" s="51"/>
+      <c r="AX48" s="34"/>
+      <c r="AY48" s="34"/>
+      <c r="AZ48" s="32"/>
+      <c r="BA48" s="51"/>
+      <c r="BB48" s="32"/>
+      <c r="BC48" s="49"/>
+      <c r="BD48" s="51"/>
+      <c r="BE48" s="32"/>
+      <c r="BF48" s="49"/>
+      <c r="BG48" s="51"/>
+      <c r="BH48" s="32"/>
+      <c r="BI48" s="51"/>
+      <c r="BJ48" s="34"/>
+      <c r="BK48" s="32"/>
+      <c r="BL48" s="49"/>
+      <c r="BM48" s="51"/>
+      <c r="BN48" s="32"/>
+      <c r="BO48" s="49"/>
+      <c r="BP48" s="49"/>
+      <c r="BQ48" s="51"/>
+      <c r="BR48" s="34"/>
+      <c r="BS48" s="48"/>
+      <c r="BT48" s="34"/>
+      <c r="BU48" s="34"/>
+      <c r="BV48" s="34"/>
+      <c r="BW48" s="32"/>
+      <c r="BX48" s="51"/>
+      <c r="BY48" s="32"/>
+      <c r="BZ48" s="51"/>
+      <c r="CA48" s="32"/>
+      <c r="CB48" s="51"/>
+      <c r="CC48" s="32"/>
+      <c r="CD48" s="51"/>
+      <c r="CE48" s="48"/>
+      <c r="CF48" s="48"/>
+      <c r="CG48" s="48"/>
+      <c r="CH48" s="48"/>
+      <c r="CI48" s="34"/>
+      <c r="CJ48" s="34"/>
+      <c r="CK48" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="CL48" s="86" t="s">
-        <v>305</v>
+      <c r="CL48" s="84" t="s">
+        <v>306</v>
       </c>
       <c r="CM48" s="93"/>
     </row>
@@ -22474,17 +22480,15 @@
       <c r="J49" s="35"/>
       <c r="K49" s="35"/>
       <c r="L49" s="35"/>
-      <c r="M49" s="42"/>
+      <c r="M49" s="98"/>
       <c r="N49" s="33"/>
-      <c r="O49" s="62"/>
+      <c r="O49" s="104"/>
       <c r="P49" s="33"/>
-      <c r="Q49" s="71">
-        <v>1</v>
-      </c>
+      <c r="Q49" s="104"/>
       <c r="R49" s="33"/>
-      <c r="S49" s="62"/>
+      <c r="S49" s="104"/>
       <c r="T49" s="33"/>
-      <c r="U49" s="62"/>
+      <c r="U49" s="104"/>
       <c r="V49" s="35"/>
       <c r="W49" s="35"/>
       <c r="X49" s="35"/>
@@ -22494,9 +22498,9 @@
       <c r="AB49" s="52"/>
       <c r="AC49" s="33"/>
       <c r="AD49" s="52"/>
-      <c r="AE49" s="42"/>
-      <c r="AF49" s="42"/>
-      <c r="AG49" s="42"/>
+      <c r="AE49" s="98"/>
+      <c r="AF49" s="98"/>
+      <c r="AG49" s="98"/>
       <c r="AH49" s="35"/>
       <c r="AI49" s="33"/>
       <c r="AJ49" s="52"/>
@@ -22534,7 +22538,7 @@
       <c r="BP49" s="50"/>
       <c r="BQ49" s="52"/>
       <c r="BR49" s="35"/>
-      <c r="BS49" s="42"/>
+      <c r="BS49" s="98"/>
       <c r="BT49" s="35"/>
       <c r="BU49" s="35"/>
       <c r="BV49" s="35"/>
@@ -22546,17 +22550,17 @@
       <c r="CB49" s="52"/>
       <c r="CC49" s="33"/>
       <c r="CD49" s="52"/>
-      <c r="CE49" s="42"/>
-      <c r="CF49" s="42"/>
-      <c r="CG49" s="42"/>
-      <c r="CH49" s="42"/>
+      <c r="CE49" s="98"/>
+      <c r="CF49" s="98"/>
+      <c r="CG49" s="98"/>
+      <c r="CH49" s="98"/>
       <c r="CI49" s="35"/>
       <c r="CJ49" s="35"/>
       <c r="CK49" s="85" t="s">
         <v>232</v>
       </c>
       <c r="CL49" s="86" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="CM49" s="93"/>
     </row>
@@ -22575,11 +22579,13 @@
       <c r="J50" s="35"/>
       <c r="K50" s="35"/>
       <c r="L50" s="35"/>
-      <c r="M50" s="35"/>
+      <c r="M50" s="42"/>
       <c r="N50" s="33"/>
-      <c r="O50" s="52"/>
+      <c r="O50" s="62"/>
       <c r="P50" s="33"/>
-      <c r="Q50" s="52"/>
+      <c r="Q50" s="71">
+        <v>1</v>
+      </c>
       <c r="R50" s="33"/>
       <c r="S50" s="62"/>
       <c r="T50" s="33"/>
@@ -22593,9 +22599,9 @@
       <c r="AB50" s="52"/>
       <c r="AC50" s="33"/>
       <c r="AD50" s="52"/>
-      <c r="AE50" s="35"/>
-      <c r="AF50" s="35"/>
-      <c r="AG50" s="35"/>
+      <c r="AE50" s="42"/>
+      <c r="AF50" s="42"/>
+      <c r="AG50" s="42"/>
       <c r="AH50" s="35"/>
       <c r="AI50" s="33"/>
       <c r="AJ50" s="52"/>
@@ -22633,7 +22639,7 @@
       <c r="BP50" s="50"/>
       <c r="BQ50" s="52"/>
       <c r="BR50" s="35"/>
-      <c r="BS50" s="35"/>
+      <c r="BS50" s="42"/>
       <c r="BT50" s="35"/>
       <c r="BU50" s="35"/>
       <c r="BV50" s="35"/>
@@ -22645,17 +22651,17 @@
       <c r="CB50" s="52"/>
       <c r="CC50" s="33"/>
       <c r="CD50" s="52"/>
-      <c r="CE50" s="35"/>
-      <c r="CF50" s="35"/>
-      <c r="CG50" s="35"/>
-      <c r="CH50" s="35"/>
+      <c r="CE50" s="42"/>
+      <c r="CF50" s="42"/>
+      <c r="CG50" s="42"/>
+      <c r="CH50" s="42"/>
       <c r="CI50" s="35"/>
       <c r="CJ50" s="35"/>
       <c r="CK50" s="85" t="s">
         <v>233</v>
       </c>
       <c r="CL50" s="86" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="CM50" s="93"/>
     </row>
@@ -22680,9 +22686,9 @@
       <c r="P51" s="33"/>
       <c r="Q51" s="52"/>
       <c r="R51" s="33"/>
-      <c r="S51" s="52"/>
+      <c r="S51" s="62"/>
       <c r="T51" s="33"/>
-      <c r="U51" s="52"/>
+      <c r="U51" s="62"/>
       <c r="V51" s="35"/>
       <c r="W51" s="35"/>
       <c r="X51" s="35"/>
@@ -22694,7 +22700,7 @@
       <c r="AD51" s="52"/>
       <c r="AE51" s="35"/>
       <c r="AF51" s="35"/>
-      <c r="AG51" s="42"/>
+      <c r="AG51" s="35"/>
       <c r="AH51" s="35"/>
       <c r="AI51" s="33"/>
       <c r="AJ51" s="52"/>
@@ -22754,7 +22760,7 @@
         <v>234</v>
       </c>
       <c r="CL51" s="86" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="CM51" s="93"/>
     </row>
@@ -22779,9 +22785,9 @@
       <c r="P52" s="33"/>
       <c r="Q52" s="52"/>
       <c r="R52" s="33"/>
-      <c r="S52" s="62"/>
+      <c r="S52" s="52"/>
       <c r="T52" s="33"/>
-      <c r="U52" s="62"/>
+      <c r="U52" s="52"/>
       <c r="V52" s="35"/>
       <c r="W52" s="35"/>
       <c r="X52" s="35"/>
@@ -22793,7 +22799,7 @@
       <c r="AD52" s="52"/>
       <c r="AE52" s="35"/>
       <c r="AF52" s="35"/>
-      <c r="AG52" s="35"/>
+      <c r="AG52" s="42"/>
       <c r="AH52" s="35"/>
       <c r="AI52" s="33"/>
       <c r="AJ52" s="52"/>
@@ -22853,7 +22859,7 @@
         <v>235</v>
       </c>
       <c r="CL52" s="86" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="CM52" s="93"/>
     </row>
@@ -22870,15 +22876,13 @@
       <c r="H53" s="35"/>
       <c r="I53" s="35"/>
       <c r="J53" s="35"/>
-      <c r="K53" s="42"/>
+      <c r="K53" s="35"/>
       <c r="L53" s="35"/>
-      <c r="M53" s="42"/>
+      <c r="M53" s="35"/>
       <c r="N53" s="33"/>
-      <c r="O53" s="62"/>
+      <c r="O53" s="52"/>
       <c r="P53" s="33"/>
-      <c r="Q53" s="71">
-        <v>1</v>
-      </c>
+      <c r="Q53" s="52"/>
       <c r="R53" s="33"/>
       <c r="S53" s="62"/>
       <c r="T53" s="33"/>
@@ -22892,9 +22896,9 @@
       <c r="AB53" s="52"/>
       <c r="AC53" s="33"/>
       <c r="AD53" s="52"/>
-      <c r="AE53" s="42"/>
-      <c r="AF53" s="42"/>
-      <c r="AG53" s="42"/>
+      <c r="AE53" s="35"/>
+      <c r="AF53" s="35"/>
+      <c r="AG53" s="35"/>
       <c r="AH53" s="35"/>
       <c r="AI53" s="33"/>
       <c r="AJ53" s="52"/>
@@ -22932,7 +22936,7 @@
       <c r="BP53" s="50"/>
       <c r="BQ53" s="52"/>
       <c r="BR53" s="35"/>
-      <c r="BS53" s="42"/>
+      <c r="BS53" s="35"/>
       <c r="BT53" s="35"/>
       <c r="BU53" s="35"/>
       <c r="BV53" s="35"/>
@@ -22944,17 +22948,17 @@
       <c r="CB53" s="52"/>
       <c r="CC53" s="33"/>
       <c r="CD53" s="52"/>
-      <c r="CE53" s="42"/>
-      <c r="CF53" s="42"/>
-      <c r="CG53" s="42"/>
-      <c r="CH53" s="42"/>
+      <c r="CE53" s="35"/>
+      <c r="CF53" s="35"/>
+      <c r="CG53" s="35"/>
+      <c r="CH53" s="35"/>
       <c r="CI53" s="35"/>
       <c r="CJ53" s="35"/>
       <c r="CK53" s="85" t="s">
         <v>236</v>
       </c>
       <c r="CL53" s="86" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="CM53" s="93"/>
     </row>
@@ -22967,21 +22971,23 @@
       <c r="D54" s="35"/>
       <c r="E54" s="35"/>
       <c r="F54" s="35"/>
-      <c r="G54" s="42"/>
+      <c r="G54" s="35"/>
       <c r="H54" s="35"/>
       <c r="I54" s="35"/>
       <c r="J54" s="35"/>
-      <c r="K54" s="35"/>
+      <c r="K54" s="42"/>
       <c r="L54" s="35"/>
-      <c r="M54" s="35"/>
+      <c r="M54" s="42"/>
       <c r="N54" s="33"/>
-      <c r="O54" s="52"/>
+      <c r="O54" s="62"/>
       <c r="P54" s="33"/>
-      <c r="Q54" s="52"/>
+      <c r="Q54" s="71">
+        <v>1</v>
+      </c>
       <c r="R54" s="33"/>
-      <c r="S54" s="52"/>
+      <c r="S54" s="62"/>
       <c r="T54" s="33"/>
-      <c r="U54" s="52"/>
+      <c r="U54" s="62"/>
       <c r="V54" s="35"/>
       <c r="W54" s="35"/>
       <c r="X54" s="35"/>
@@ -22992,18 +22998,18 @@
       <c r="AC54" s="33"/>
       <c r="AD54" s="52"/>
       <c r="AE54" s="42"/>
-      <c r="AF54" s="35"/>
+      <c r="AF54" s="42"/>
       <c r="AG54" s="42"/>
       <c r="AH54" s="35"/>
       <c r="AI54" s="33"/>
       <c r="AJ54" s="52"/>
       <c r="AK54" s="33"/>
       <c r="AL54" s="52"/>
-      <c r="AM54" s="61"/>
-      <c r="AN54" s="75"/>
+      <c r="AM54" s="33"/>
+      <c r="AN54" s="50"/>
       <c r="AO54" s="52"/>
-      <c r="AP54" s="61"/>
-      <c r="AQ54" s="75"/>
+      <c r="AP54" s="33"/>
+      <c r="AQ54" s="50"/>
       <c r="AR54" s="52"/>
       <c r="AS54" s="35"/>
       <c r="AT54" s="35"/>
@@ -23031,7 +23037,7 @@
       <c r="BP54" s="50"/>
       <c r="BQ54" s="52"/>
       <c r="BR54" s="35"/>
-      <c r="BS54" s="35"/>
+      <c r="BS54" s="42"/>
       <c r="BT54" s="35"/>
       <c r="BU54" s="35"/>
       <c r="BV54" s="35"/>
@@ -23053,7 +23059,7 @@
         <v>237</v>
       </c>
       <c r="CL54" s="86" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="CM54" s="93"/>
     </row>
@@ -23099,10 +23105,10 @@
       <c r="AK55" s="33"/>
       <c r="AL55" s="52"/>
       <c r="AM55" s="61"/>
-      <c r="AN55" s="50"/>
+      <c r="AN55" s="75"/>
       <c r="AO55" s="52"/>
       <c r="AP55" s="61"/>
-      <c r="AQ55" s="50"/>
+      <c r="AQ55" s="75"/>
       <c r="AR55" s="52"/>
       <c r="AS55" s="35"/>
       <c r="AT55" s="35"/>
@@ -23152,7 +23158,7 @@
         <v>238</v>
       </c>
       <c r="CL55" s="86" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="CM55" s="93"/>
     </row>
@@ -23165,13 +23171,11 @@
       <c r="D56" s="35"/>
       <c r="E56" s="35"/>
       <c r="F56" s="35"/>
-      <c r="G56" s="35"/>
+      <c r="G56" s="42"/>
       <c r="H56" s="35"/>
       <c r="I56" s="35"/>
       <c r="J56" s="35"/>
-      <c r="K56" s="101">
-        <v>3</v>
-      </c>
+      <c r="K56" s="35"/>
       <c r="L56" s="35"/>
       <c r="M56" s="35"/>
       <c r="N56" s="33"/>
@@ -23191,18 +23195,18 @@
       <c r="AB56" s="52"/>
       <c r="AC56" s="33"/>
       <c r="AD56" s="52"/>
-      <c r="AE56" s="98"/>
+      <c r="AE56" s="42"/>
       <c r="AF56" s="35"/>
-      <c r="AG56" s="98"/>
+      <c r="AG56" s="42"/>
       <c r="AH56" s="35"/>
       <c r="AI56" s="33"/>
       <c r="AJ56" s="52"/>
       <c r="AK56" s="33"/>
       <c r="AL56" s="52"/>
-      <c r="AM56" s="33"/>
+      <c r="AM56" s="61"/>
       <c r="AN56" s="50"/>
       <c r="AO56" s="52"/>
-      <c r="AP56" s="33"/>
+      <c r="AP56" s="61"/>
       <c r="AQ56" s="50"/>
       <c r="AR56" s="52"/>
       <c r="AS56" s="35"/>
@@ -23243,17 +23247,17 @@
       <c r="CB56" s="52"/>
       <c r="CC56" s="33"/>
       <c r="CD56" s="52"/>
-      <c r="CE56" s="98"/>
-      <c r="CF56" s="98"/>
-      <c r="CG56" s="98"/>
-      <c r="CH56" s="98"/>
+      <c r="CE56" s="42"/>
+      <c r="CF56" s="42"/>
+      <c r="CG56" s="42"/>
+      <c r="CH56" s="42"/>
       <c r="CI56" s="35"/>
       <c r="CJ56" s="35"/>
       <c r="CK56" s="85" t="s">
         <v>239</v>
       </c>
       <c r="CL56" s="86" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="CM56" s="93"/>
     </row>
@@ -23270,7 +23274,9 @@
       <c r="H57" s="35"/>
       <c r="I57" s="35"/>
       <c r="J57" s="35"/>
-      <c r="K57" s="35"/>
+      <c r="K57" s="101">
+        <v>3</v>
+      </c>
       <c r="L57" s="35"/>
       <c r="M57" s="35"/>
       <c r="N57" s="33"/>
@@ -23290,11 +23296,9 @@
       <c r="AB57" s="52"/>
       <c r="AC57" s="33"/>
       <c r="AD57" s="52"/>
-      <c r="AE57" s="35"/>
-      <c r="AF57" s="101">
-        <v>2</v>
-      </c>
-      <c r="AG57" s="35"/>
+      <c r="AE57" s="98"/>
+      <c r="AF57" s="35"/>
+      <c r="AG57" s="98"/>
       <c r="AH57" s="35"/>
       <c r="AI57" s="33"/>
       <c r="AJ57" s="52"/>
@@ -23344,316 +23348,318 @@
       <c r="CB57" s="52"/>
       <c r="CC57" s="33"/>
       <c r="CD57" s="52"/>
-      <c r="CE57" s="35"/>
-      <c r="CF57" s="35"/>
-      <c r="CG57" s="35"/>
-      <c r="CH57" s="35"/>
+      <c r="CE57" s="98"/>
+      <c r="CF57" s="98"/>
+      <c r="CG57" s="98"/>
+      <c r="CH57" s="98"/>
       <c r="CI57" s="35"/>
       <c r="CJ57" s="35"/>
       <c r="CK57" s="85" t="s">
         <v>240</v>
       </c>
       <c r="CL57" s="86" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="CM57" s="93"/>
     </row>
-    <row r="58" spans="1:91" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A58" s="93"/>
-      <c r="B58" s="17"/>
-      <c r="C58" s="88" t="s">
+      <c r="B58" s="16"/>
+      <c r="C58" s="86" t="s">
         <v>241</v>
       </c>
-      <c r="D58" s="36"/>
-      <c r="E58" s="36"/>
-      <c r="F58" s="36"/>
-      <c r="G58" s="36"/>
-      <c r="H58" s="36"/>
-      <c r="I58" s="36"/>
-      <c r="J58" s="36"/>
-      <c r="K58" s="36"/>
-      <c r="L58" s="36"/>
-      <c r="M58" s="36"/>
-      <c r="N58" s="53"/>
-      <c r="O58" s="54"/>
-      <c r="P58" s="53"/>
-      <c r="Q58" s="54"/>
-      <c r="R58" s="53"/>
-      <c r="S58" s="54"/>
-      <c r="T58" s="53"/>
-      <c r="U58" s="54"/>
-      <c r="V58" s="36"/>
-      <c r="W58" s="36"/>
-      <c r="X58" s="36"/>
-      <c r="Y58" s="53"/>
-      <c r="Z58" s="54"/>
-      <c r="AA58" s="53"/>
-      <c r="AB58" s="54"/>
-      <c r="AC58" s="53"/>
-      <c r="AD58" s="54"/>
-      <c r="AE58" s="36"/>
-      <c r="AF58" s="36"/>
-      <c r="AG58" s="36"/>
-      <c r="AH58" s="36"/>
-      <c r="AI58" s="53"/>
-      <c r="AJ58" s="54"/>
-      <c r="AK58" s="53"/>
-      <c r="AL58" s="54"/>
-      <c r="AM58" s="53"/>
-      <c r="AN58" s="73"/>
-      <c r="AO58" s="54"/>
-      <c r="AP58" s="53"/>
-      <c r="AQ58" s="73"/>
-      <c r="AR58" s="54"/>
-      <c r="AS58" s="36"/>
-      <c r="AT58" s="36"/>
-      <c r="AU58" s="36"/>
-      <c r="AV58" s="53"/>
-      <c r="AW58" s="54"/>
-      <c r="AX58" s="36"/>
-      <c r="AY58" s="36"/>
-      <c r="AZ58" s="53"/>
-      <c r="BA58" s="54"/>
-      <c r="BB58" s="53"/>
-      <c r="BC58" s="73"/>
-      <c r="BD58" s="54"/>
-      <c r="BE58" s="53"/>
-      <c r="BF58" s="73"/>
-      <c r="BG58" s="54"/>
-      <c r="BH58" s="53"/>
-      <c r="BI58" s="54"/>
-      <c r="BJ58" s="36"/>
-      <c r="BK58" s="53"/>
-      <c r="BL58" s="73"/>
-      <c r="BM58" s="54"/>
-      <c r="BN58" s="53"/>
-      <c r="BO58" s="73"/>
-      <c r="BP58" s="73"/>
-      <c r="BQ58" s="54"/>
-      <c r="BR58" s="36"/>
-      <c r="BS58" s="36"/>
-      <c r="BT58" s="36"/>
-      <c r="BU58" s="36"/>
-      <c r="BV58" s="36"/>
-      <c r="BW58" s="53"/>
-      <c r="BX58" s="54"/>
-      <c r="BY58" s="53"/>
-      <c r="BZ58" s="54"/>
-      <c r="CA58" s="53"/>
-      <c r="CB58" s="54"/>
-      <c r="CC58" s="53"/>
-      <c r="CD58" s="54"/>
-      <c r="CE58" s="36"/>
-      <c r="CF58" s="36"/>
-      <c r="CG58" s="36"/>
-      <c r="CH58" s="36"/>
-      <c r="CI58" s="36"/>
-      <c r="CJ58" s="36"/>
-      <c r="CK58" s="87" t="s">
+      <c r="D58" s="35"/>
+      <c r="E58" s="35"/>
+      <c r="F58" s="35"/>
+      <c r="G58" s="35"/>
+      <c r="H58" s="35"/>
+      <c r="I58" s="35"/>
+      <c r="J58" s="35"/>
+      <c r="K58" s="35"/>
+      <c r="L58" s="35"/>
+      <c r="M58" s="35"/>
+      <c r="N58" s="33"/>
+      <c r="O58" s="52"/>
+      <c r="P58" s="33"/>
+      <c r="Q58" s="52"/>
+      <c r="R58" s="33"/>
+      <c r="S58" s="52"/>
+      <c r="T58" s="33"/>
+      <c r="U58" s="52"/>
+      <c r="V58" s="35"/>
+      <c r="W58" s="35"/>
+      <c r="X58" s="35"/>
+      <c r="Y58" s="33"/>
+      <c r="Z58" s="52"/>
+      <c r="AA58" s="33"/>
+      <c r="AB58" s="52"/>
+      <c r="AC58" s="33"/>
+      <c r="AD58" s="52"/>
+      <c r="AE58" s="35"/>
+      <c r="AF58" s="101">
+        <v>2</v>
+      </c>
+      <c r="AG58" s="35"/>
+      <c r="AH58" s="35"/>
+      <c r="AI58" s="33"/>
+      <c r="AJ58" s="52"/>
+      <c r="AK58" s="33"/>
+      <c r="AL58" s="52"/>
+      <c r="AM58" s="33"/>
+      <c r="AN58" s="50"/>
+      <c r="AO58" s="52"/>
+      <c r="AP58" s="33"/>
+      <c r="AQ58" s="50"/>
+      <c r="AR58" s="52"/>
+      <c r="AS58" s="35"/>
+      <c r="AT58" s="35"/>
+      <c r="AU58" s="35"/>
+      <c r="AV58" s="33"/>
+      <c r="AW58" s="52"/>
+      <c r="AX58" s="35"/>
+      <c r="AY58" s="35"/>
+      <c r="AZ58" s="33"/>
+      <c r="BA58" s="52"/>
+      <c r="BB58" s="33"/>
+      <c r="BC58" s="50"/>
+      <c r="BD58" s="52"/>
+      <c r="BE58" s="33"/>
+      <c r="BF58" s="50"/>
+      <c r="BG58" s="52"/>
+      <c r="BH58" s="33"/>
+      <c r="BI58" s="52"/>
+      <c r="BJ58" s="35"/>
+      <c r="BK58" s="33"/>
+      <c r="BL58" s="50"/>
+      <c r="BM58" s="52"/>
+      <c r="BN58" s="33"/>
+      <c r="BO58" s="50"/>
+      <c r="BP58" s="50"/>
+      <c r="BQ58" s="52"/>
+      <c r="BR58" s="35"/>
+      <c r="BS58" s="35"/>
+      <c r="BT58" s="35"/>
+      <c r="BU58" s="35"/>
+      <c r="BV58" s="35"/>
+      <c r="BW58" s="33"/>
+      <c r="BX58" s="52"/>
+      <c r="BY58" s="33"/>
+      <c r="BZ58" s="52"/>
+      <c r="CA58" s="33"/>
+      <c r="CB58" s="52"/>
+      <c r="CC58" s="33"/>
+      <c r="CD58" s="52"/>
+      <c r="CE58" s="35"/>
+      <c r="CF58" s="35"/>
+      <c r="CG58" s="35"/>
+      <c r="CH58" s="35"/>
+      <c r="CI58" s="35"/>
+      <c r="CJ58" s="35"/>
+      <c r="CK58" s="85" t="s">
         <v>241</v>
       </c>
-      <c r="CL58" s="88" t="s">
-        <v>315</v>
+      <c r="CL58" s="86" t="s">
+        <v>316</v>
       </c>
       <c r="CM58" s="93"/>
     </row>
-    <row r="59" spans="1:91" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:91" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" s="93"/>
-      <c r="B59" s="29" t="s">
+      <c r="B59" s="17"/>
+      <c r="C59" s="88" t="s">
         <v>242</v>
       </c>
-      <c r="C59" s="89" t="s">
-        <v>243</v>
-      </c>
-      <c r="D59" s="39"/>
-      <c r="E59" s="39"/>
-      <c r="F59" s="39"/>
-      <c r="G59" s="39"/>
-      <c r="H59" s="39"/>
-      <c r="I59" s="39"/>
-      <c r="J59" s="39"/>
-      <c r="K59" s="39"/>
-      <c r="L59" s="39"/>
-      <c r="M59" s="39"/>
-      <c r="N59" s="37"/>
-      <c r="O59" s="57"/>
-      <c r="P59" s="37"/>
-      <c r="Q59" s="57"/>
-      <c r="R59" s="37"/>
-      <c r="S59" s="57"/>
-      <c r="T59" s="37"/>
-      <c r="U59" s="57"/>
-      <c r="V59" s="39"/>
-      <c r="W59" s="39"/>
-      <c r="X59" s="39"/>
-      <c r="Y59" s="37"/>
-      <c r="Z59" s="57"/>
-      <c r="AA59" s="37"/>
-      <c r="AB59" s="57"/>
-      <c r="AC59" s="37"/>
-      <c r="AD59" s="57"/>
-      <c r="AE59" s="39"/>
-      <c r="AF59" s="39"/>
-      <c r="AG59" s="39"/>
-      <c r="AH59" s="39"/>
-      <c r="AI59" s="37"/>
-      <c r="AJ59" s="57"/>
-      <c r="AK59" s="37"/>
-      <c r="AL59" s="57"/>
-      <c r="AM59" s="37"/>
-      <c r="AN59" s="55"/>
-      <c r="AO59" s="57"/>
-      <c r="AP59" s="37"/>
-      <c r="AQ59" s="55"/>
-      <c r="AR59" s="57"/>
-      <c r="AS59" s="39"/>
-      <c r="AT59" s="39"/>
-      <c r="AU59" s="39"/>
-      <c r="AV59" s="37"/>
-      <c r="AW59" s="57"/>
-      <c r="AX59" s="39"/>
-      <c r="AY59" s="39"/>
-      <c r="AZ59" s="37"/>
-      <c r="BA59" s="57"/>
-      <c r="BB59" s="37"/>
-      <c r="BC59" s="55"/>
-      <c r="BD59" s="57"/>
-      <c r="BE59" s="37"/>
-      <c r="BF59" s="55"/>
-      <c r="BG59" s="57"/>
-      <c r="BH59" s="37"/>
-      <c r="BI59" s="57"/>
-      <c r="BJ59" s="39"/>
-      <c r="BK59" s="37"/>
-      <c r="BL59" s="55"/>
-      <c r="BM59" s="57"/>
-      <c r="BN59" s="37"/>
-      <c r="BO59" s="55"/>
-      <c r="BP59" s="55"/>
-      <c r="BQ59" s="57"/>
-      <c r="BR59" s="39"/>
-      <c r="BS59" s="39"/>
-      <c r="BT59" s="39"/>
-      <c r="BU59" s="48"/>
-      <c r="BV59" s="39"/>
-      <c r="BW59" s="80"/>
-      <c r="BX59" s="57"/>
-      <c r="BY59" s="80"/>
-      <c r="BZ59" s="57"/>
-      <c r="CA59" s="37"/>
-      <c r="CB59" s="57"/>
-      <c r="CC59" s="37"/>
-      <c r="CD59" s="57"/>
-      <c r="CE59" s="39"/>
-      <c r="CF59" s="39"/>
-      <c r="CG59" s="39"/>
-      <c r="CH59" s="39"/>
-      <c r="CI59" s="39"/>
-      <c r="CJ59" s="39"/>
-      <c r="CK59" s="18" t="s">
-        <v>243</v>
-      </c>
-      <c r="CL59" s="89" t="s">
-        <v>316</v>
+      <c r="D59" s="36"/>
+      <c r="E59" s="36"/>
+      <c r="F59" s="36"/>
+      <c r="G59" s="36"/>
+      <c r="H59" s="36"/>
+      <c r="I59" s="36"/>
+      <c r="J59" s="36"/>
+      <c r="K59" s="36"/>
+      <c r="L59" s="36"/>
+      <c r="M59" s="36"/>
+      <c r="N59" s="53"/>
+      <c r="O59" s="54"/>
+      <c r="P59" s="53"/>
+      <c r="Q59" s="54"/>
+      <c r="R59" s="53"/>
+      <c r="S59" s="54"/>
+      <c r="T59" s="53"/>
+      <c r="U59" s="54"/>
+      <c r="V59" s="36"/>
+      <c r="W59" s="36"/>
+      <c r="X59" s="36"/>
+      <c r="Y59" s="53"/>
+      <c r="Z59" s="54"/>
+      <c r="AA59" s="53"/>
+      <c r="AB59" s="54"/>
+      <c r="AC59" s="53"/>
+      <c r="AD59" s="54"/>
+      <c r="AE59" s="36"/>
+      <c r="AF59" s="36"/>
+      <c r="AG59" s="36"/>
+      <c r="AH59" s="36"/>
+      <c r="AI59" s="53"/>
+      <c r="AJ59" s="54"/>
+      <c r="AK59" s="53"/>
+      <c r="AL59" s="54"/>
+      <c r="AM59" s="53"/>
+      <c r="AN59" s="73"/>
+      <c r="AO59" s="54"/>
+      <c r="AP59" s="53"/>
+      <c r="AQ59" s="73"/>
+      <c r="AR59" s="54"/>
+      <c r="AS59" s="36"/>
+      <c r="AT59" s="36"/>
+      <c r="AU59" s="36"/>
+      <c r="AV59" s="53"/>
+      <c r="AW59" s="54"/>
+      <c r="AX59" s="36"/>
+      <c r="AY59" s="36"/>
+      <c r="AZ59" s="53"/>
+      <c r="BA59" s="54"/>
+      <c r="BB59" s="53"/>
+      <c r="BC59" s="73"/>
+      <c r="BD59" s="54"/>
+      <c r="BE59" s="53"/>
+      <c r="BF59" s="73"/>
+      <c r="BG59" s="54"/>
+      <c r="BH59" s="53"/>
+      <c r="BI59" s="54"/>
+      <c r="BJ59" s="36"/>
+      <c r="BK59" s="53"/>
+      <c r="BL59" s="73"/>
+      <c r="BM59" s="54"/>
+      <c r="BN59" s="53"/>
+      <c r="BO59" s="73"/>
+      <c r="BP59" s="73"/>
+      <c r="BQ59" s="54"/>
+      <c r="BR59" s="36"/>
+      <c r="BS59" s="36"/>
+      <c r="BT59" s="36"/>
+      <c r="BU59" s="36"/>
+      <c r="BV59" s="36"/>
+      <c r="BW59" s="53"/>
+      <c r="BX59" s="54"/>
+      <c r="BY59" s="53"/>
+      <c r="BZ59" s="54"/>
+      <c r="CA59" s="53"/>
+      <c r="CB59" s="54"/>
+      <c r="CC59" s="53"/>
+      <c r="CD59" s="54"/>
+      <c r="CE59" s="36"/>
+      <c r="CF59" s="36"/>
+      <c r="CG59" s="36"/>
+      <c r="CH59" s="36"/>
+      <c r="CI59" s="36"/>
+      <c r="CJ59" s="36"/>
+      <c r="CK59" s="87" t="s">
+        <v>242</v>
+      </c>
+      <c r="CL59" s="88" t="s">
+        <v>317</v>
       </c>
       <c r="CM59" s="93"/>
     </row>
     <row r="60" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A60" s="93"/>
-      <c r="B60" s="30"/>
-      <c r="C60" s="25" t="s">
+      <c r="B60" s="29" t="s">
+        <v>243</v>
+      </c>
+      <c r="C60" s="89" t="s">
         <v>244</v>
       </c>
-      <c r="D60" s="40"/>
-      <c r="E60" s="40"/>
-      <c r="F60" s="40"/>
-      <c r="G60" s="40"/>
-      <c r="H60" s="40"/>
-      <c r="I60" s="40"/>
-      <c r="J60" s="40"/>
-      <c r="K60" s="40"/>
-      <c r="L60" s="40"/>
-      <c r="M60" s="40"/>
-      <c r="N60" s="38"/>
-      <c r="O60" s="58"/>
-      <c r="P60" s="38"/>
-      <c r="Q60" s="58"/>
-      <c r="R60" s="38"/>
-      <c r="S60" s="58"/>
-      <c r="T60" s="38"/>
-      <c r="U60" s="58"/>
-      <c r="V60" s="40"/>
-      <c r="W60" s="40"/>
-      <c r="X60" s="40"/>
-      <c r="Y60" s="38"/>
-      <c r="Z60" s="58"/>
-      <c r="AA60" s="38"/>
-      <c r="AB60" s="58"/>
-      <c r="AC60" s="38"/>
-      <c r="AD60" s="58"/>
-      <c r="AE60" s="40"/>
-      <c r="AF60" s="40"/>
-      <c r="AG60" s="40"/>
-      <c r="AH60" s="40"/>
-      <c r="AI60" s="38"/>
-      <c r="AJ60" s="58"/>
-      <c r="AK60" s="38"/>
-      <c r="AL60" s="58"/>
-      <c r="AM60" s="38"/>
-      <c r="AN60" s="56"/>
-      <c r="AO60" s="58"/>
-      <c r="AP60" s="38"/>
-      <c r="AQ60" s="56"/>
-      <c r="AR60" s="58"/>
-      <c r="AS60" s="40"/>
-      <c r="AT60" s="40"/>
-      <c r="AU60" s="40"/>
-      <c r="AV60" s="38"/>
-      <c r="AW60" s="58"/>
-      <c r="AX60" s="40"/>
-      <c r="AY60" s="40"/>
-      <c r="AZ60" s="38"/>
-      <c r="BA60" s="58"/>
-      <c r="BB60" s="38"/>
-      <c r="BC60" s="56"/>
-      <c r="BD60" s="58"/>
-      <c r="BE60" s="38"/>
-      <c r="BF60" s="56"/>
-      <c r="BG60" s="58"/>
-      <c r="BH60" s="38"/>
-      <c r="BI60" s="58"/>
-      <c r="BJ60" s="40"/>
-      <c r="BK60" s="38"/>
-      <c r="BL60" s="56"/>
-      <c r="BM60" s="58"/>
-      <c r="BN60" s="38"/>
-      <c r="BO60" s="56"/>
-      <c r="BP60" s="56"/>
-      <c r="BQ60" s="58"/>
-      <c r="BR60" s="40"/>
-      <c r="BS60" s="40"/>
-      <c r="BT60" s="40"/>
-      <c r="BU60" s="40"/>
-      <c r="BV60" s="40"/>
-      <c r="BW60" s="38"/>
-      <c r="BX60" s="58"/>
-      <c r="BY60" s="38"/>
-      <c r="BZ60" s="58"/>
-      <c r="CA60" s="38"/>
-      <c r="CB60" s="58"/>
-      <c r="CC60" s="38"/>
-      <c r="CD60" s="58"/>
-      <c r="CE60" s="40"/>
-      <c r="CF60" s="40"/>
-      <c r="CG60" s="40"/>
-      <c r="CH60" s="40"/>
-      <c r="CI60" s="40"/>
-      <c r="CJ60" s="40"/>
-      <c r="CK60" s="90" t="s">
+      <c r="D60" s="39"/>
+      <c r="E60" s="39"/>
+      <c r="F60" s="39"/>
+      <c r="G60" s="39"/>
+      <c r="H60" s="39"/>
+      <c r="I60" s="39"/>
+      <c r="J60" s="39"/>
+      <c r="K60" s="39"/>
+      <c r="L60" s="39"/>
+      <c r="M60" s="39"/>
+      <c r="N60" s="37"/>
+      <c r="O60" s="57"/>
+      <c r="P60" s="37"/>
+      <c r="Q60" s="57"/>
+      <c r="R60" s="37"/>
+      <c r="S60" s="57"/>
+      <c r="T60" s="37"/>
+      <c r="U60" s="57"/>
+      <c r="V60" s="39"/>
+      <c r="W60" s="39"/>
+      <c r="X60" s="39"/>
+      <c r="Y60" s="37"/>
+      <c r="Z60" s="57"/>
+      <c r="AA60" s="37"/>
+      <c r="AB60" s="57"/>
+      <c r="AC60" s="37"/>
+      <c r="AD60" s="57"/>
+      <c r="AE60" s="39"/>
+      <c r="AF60" s="39"/>
+      <c r="AG60" s="39"/>
+      <c r="AH60" s="39"/>
+      <c r="AI60" s="37"/>
+      <c r="AJ60" s="57"/>
+      <c r="AK60" s="37"/>
+      <c r="AL60" s="57"/>
+      <c r="AM60" s="37"/>
+      <c r="AN60" s="55"/>
+      <c r="AO60" s="57"/>
+      <c r="AP60" s="37"/>
+      <c r="AQ60" s="55"/>
+      <c r="AR60" s="57"/>
+      <c r="AS60" s="39"/>
+      <c r="AT60" s="39"/>
+      <c r="AU60" s="39"/>
+      <c r="AV60" s="37"/>
+      <c r="AW60" s="57"/>
+      <c r="AX60" s="39"/>
+      <c r="AY60" s="39"/>
+      <c r="AZ60" s="37"/>
+      <c r="BA60" s="57"/>
+      <c r="BB60" s="37"/>
+      <c r="BC60" s="55"/>
+      <c r="BD60" s="57"/>
+      <c r="BE60" s="37"/>
+      <c r="BF60" s="55"/>
+      <c r="BG60" s="57"/>
+      <c r="BH60" s="37"/>
+      <c r="BI60" s="57"/>
+      <c r="BJ60" s="39"/>
+      <c r="BK60" s="37"/>
+      <c r="BL60" s="55"/>
+      <c r="BM60" s="57"/>
+      <c r="BN60" s="37"/>
+      <c r="BO60" s="55"/>
+      <c r="BP60" s="55"/>
+      <c r="BQ60" s="57"/>
+      <c r="BR60" s="39"/>
+      <c r="BS60" s="39"/>
+      <c r="BT60" s="39"/>
+      <c r="BU60" s="48"/>
+      <c r="BV60" s="39"/>
+      <c r="BW60" s="80"/>
+      <c r="BX60" s="57"/>
+      <c r="BY60" s="80"/>
+      <c r="BZ60" s="57"/>
+      <c r="CA60" s="37"/>
+      <c r="CB60" s="57"/>
+      <c r="CC60" s="37"/>
+      <c r="CD60" s="57"/>
+      <c r="CE60" s="39"/>
+      <c r="CF60" s="39"/>
+      <c r="CG60" s="39"/>
+      <c r="CH60" s="39"/>
+      <c r="CI60" s="39"/>
+      <c r="CJ60" s="39"/>
+      <c r="CK60" s="18" t="s">
         <v>244</v>
       </c>
-      <c r="CL60" s="25" t="s">
-        <v>317</v>
+      <c r="CL60" s="89" t="s">
+        <v>318</v>
       </c>
       <c r="CM60" s="93"/>
     </row>
@@ -23693,7 +23699,7 @@
       <c r="AE61" s="40"/>
       <c r="AF61" s="40"/>
       <c r="AG61" s="40"/>
-      <c r="AH61" s="42"/>
+      <c r="AH61" s="40"/>
       <c r="AI61" s="38"/>
       <c r="AJ61" s="58"/>
       <c r="AK61" s="38"/>
@@ -23752,7 +23758,7 @@
         <v>245</v>
       </c>
       <c r="CL61" s="25" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="CM61" s="93"/>
     </row>
@@ -23792,7 +23798,7 @@
       <c r="AE62" s="40"/>
       <c r="AF62" s="40"/>
       <c r="AG62" s="40"/>
-      <c r="AH62" s="40"/>
+      <c r="AH62" s="42"/>
       <c r="AI62" s="38"/>
       <c r="AJ62" s="58"/>
       <c r="AK62" s="38"/>
@@ -23851,7 +23857,7 @@
         <v>246</v>
       </c>
       <c r="CL62" s="25" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="CM62" s="93"/>
     </row>
@@ -23891,9 +23897,9 @@
       <c r="AE63" s="40"/>
       <c r="AF63" s="40"/>
       <c r="AG63" s="40"/>
-      <c r="AH63" s="42"/>
+      <c r="AH63" s="40"/>
       <c r="AI63" s="38"/>
-      <c r="AJ63" s="62"/>
+      <c r="AJ63" s="58"/>
       <c r="AK63" s="38"/>
       <c r="AL63" s="58"/>
       <c r="AM63" s="38"/>
@@ -23902,8 +23908,8 @@
       <c r="AP63" s="38"/>
       <c r="AQ63" s="56"/>
       <c r="AR63" s="58"/>
-      <c r="AS63" s="42"/>
-      <c r="AT63" s="42"/>
+      <c r="AS63" s="40"/>
+      <c r="AT63" s="40"/>
       <c r="AU63" s="40"/>
       <c r="AV63" s="38"/>
       <c r="AW63" s="58"/>
@@ -23936,7 +23942,7 @@
       <c r="BX63" s="58"/>
       <c r="BY63" s="38"/>
       <c r="BZ63" s="58"/>
-      <c r="CA63" s="61"/>
+      <c r="CA63" s="38"/>
       <c r="CB63" s="58"/>
       <c r="CC63" s="38"/>
       <c r="CD63" s="58"/>
@@ -23950,7 +23956,7 @@
         <v>247</v>
       </c>
       <c r="CL63" s="25" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="CM63" s="93"/>
     </row>
@@ -23963,7 +23969,7 @@
       <c r="D64" s="40"/>
       <c r="E64" s="40"/>
       <c r="F64" s="40"/>
-      <c r="G64" s="42"/>
+      <c r="G64" s="40"/>
       <c r="H64" s="40"/>
       <c r="I64" s="40"/>
       <c r="J64" s="40"/>
@@ -23990,19 +23996,19 @@
       <c r="AE64" s="40"/>
       <c r="AF64" s="40"/>
       <c r="AG64" s="40"/>
-      <c r="AH64" s="40"/>
+      <c r="AH64" s="42"/>
       <c r="AI64" s="38"/>
-      <c r="AJ64" s="58"/>
+      <c r="AJ64" s="62"/>
       <c r="AK64" s="38"/>
       <c r="AL64" s="58"/>
-      <c r="AM64" s="61"/>
-      <c r="AN64" s="75"/>
+      <c r="AM64" s="38"/>
+      <c r="AN64" s="56"/>
       <c r="AO64" s="58"/>
-      <c r="AP64" s="61"/>
-      <c r="AQ64" s="75"/>
+      <c r="AP64" s="38"/>
+      <c r="AQ64" s="56"/>
       <c r="AR64" s="58"/>
-      <c r="AS64" s="40"/>
-      <c r="AT64" s="40"/>
+      <c r="AS64" s="42"/>
+      <c r="AT64" s="42"/>
       <c r="AU64" s="40"/>
       <c r="AV64" s="38"/>
       <c r="AW64" s="58"/>
@@ -24035,7 +24041,7 @@
       <c r="BX64" s="58"/>
       <c r="BY64" s="38"/>
       <c r="BZ64" s="58"/>
-      <c r="CA64" s="38"/>
+      <c r="CA64" s="61"/>
       <c r="CB64" s="58"/>
       <c r="CC64" s="38"/>
       <c r="CD64" s="58"/>
@@ -24049,7 +24055,7 @@
         <v>248</v>
       </c>
       <c r="CL64" s="25" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="CM64" s="93"/>
     </row>
@@ -24148,7 +24154,7 @@
         <v>249</v>
       </c>
       <c r="CL65" s="25" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="CM65" s="93"/>
     </row>
@@ -24161,7 +24167,7 @@
       <c r="D66" s="40"/>
       <c r="E66" s="40"/>
       <c r="F66" s="40"/>
-      <c r="G66" s="40"/>
+      <c r="G66" s="42"/>
       <c r="H66" s="40"/>
       <c r="I66" s="40"/>
       <c r="J66" s="40"/>
@@ -24188,19 +24194,19 @@
       <c r="AE66" s="40"/>
       <c r="AF66" s="40"/>
       <c r="AG66" s="40"/>
-      <c r="AH66" s="42"/>
-      <c r="AI66" s="61"/>
+      <c r="AH66" s="40"/>
+      <c r="AI66" s="38"/>
       <c r="AJ66" s="58"/>
       <c r="AK66" s="38"/>
       <c r="AL66" s="58"/>
-      <c r="AM66" s="38"/>
-      <c r="AN66" s="56"/>
+      <c r="AM66" s="61"/>
+      <c r="AN66" s="75"/>
       <c r="AO66" s="58"/>
-      <c r="AP66" s="38"/>
-      <c r="AQ66" s="56"/>
+      <c r="AP66" s="61"/>
+      <c r="AQ66" s="75"/>
       <c r="AR66" s="58"/>
-      <c r="AS66" s="42"/>
-      <c r="AT66" s="42"/>
+      <c r="AS66" s="40"/>
+      <c r="AT66" s="40"/>
       <c r="AU66" s="40"/>
       <c r="AV66" s="38"/>
       <c r="AW66" s="58"/>
@@ -24228,12 +24234,12 @@
       <c r="BS66" s="40"/>
       <c r="BT66" s="40"/>
       <c r="BU66" s="40"/>
-      <c r="BV66" s="42"/>
+      <c r="BV66" s="40"/>
       <c r="BW66" s="38"/>
       <c r="BX66" s="58"/>
       <c r="BY66" s="38"/>
       <c r="BZ66" s="58"/>
-      <c r="CA66" s="61"/>
+      <c r="CA66" s="38"/>
       <c r="CB66" s="58"/>
       <c r="CC66" s="38"/>
       <c r="CD66" s="58"/>
@@ -24247,7 +24253,7 @@
         <v>250</v>
       </c>
       <c r="CL66" s="25" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="CM66" s="93"/>
     </row>
@@ -24288,8 +24294,8 @@
       <c r="AF67" s="40"/>
       <c r="AG67" s="40"/>
       <c r="AH67" s="42"/>
-      <c r="AI67" s="38"/>
-      <c r="AJ67" s="62"/>
+      <c r="AI67" s="61"/>
+      <c r="AJ67" s="58"/>
       <c r="AK67" s="38"/>
       <c r="AL67" s="58"/>
       <c r="AM67" s="38"/>
@@ -24327,7 +24333,7 @@
       <c r="BS67" s="40"/>
       <c r="BT67" s="40"/>
       <c r="BU67" s="40"/>
-      <c r="BV67" s="40"/>
+      <c r="BV67" s="42"/>
       <c r="BW67" s="38"/>
       <c r="BX67" s="58"/>
       <c r="BY67" s="38"/>
@@ -24346,7 +24352,7 @@
         <v>251</v>
       </c>
       <c r="CL67" s="25" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="CM67" s="93"/>
     </row>
@@ -24386,9 +24392,9 @@
       <c r="AE68" s="40"/>
       <c r="AF68" s="40"/>
       <c r="AG68" s="40"/>
-      <c r="AH68" s="98"/>
+      <c r="AH68" s="42"/>
       <c r="AI68" s="38"/>
-      <c r="AJ68" s="104"/>
+      <c r="AJ68" s="62"/>
       <c r="AK68" s="38"/>
       <c r="AL68" s="58"/>
       <c r="AM68" s="38"/>
@@ -24397,8 +24403,8 @@
       <c r="AP68" s="38"/>
       <c r="AQ68" s="56"/>
       <c r="AR68" s="58"/>
-      <c r="AS68" s="40"/>
-      <c r="AT68" s="40"/>
+      <c r="AS68" s="42"/>
+      <c r="AT68" s="42"/>
       <c r="AU68" s="40"/>
       <c r="AV68" s="38"/>
       <c r="AW68" s="58"/>
@@ -24431,7 +24437,7 @@
       <c r="BX68" s="58"/>
       <c r="BY68" s="38"/>
       <c r="BZ68" s="58"/>
-      <c r="CA68" s="38"/>
+      <c r="CA68" s="61"/>
       <c r="CB68" s="58"/>
       <c r="CC68" s="38"/>
       <c r="CD68" s="58"/>
@@ -24445,7 +24451,7 @@
         <v>252</v>
       </c>
       <c r="CL68" s="25" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="CM68" s="93"/>
     </row>
@@ -24487,7 +24493,7 @@
       <c r="AG69" s="40"/>
       <c r="AH69" s="98"/>
       <c r="AI69" s="38"/>
-      <c r="AJ69" s="58"/>
+      <c r="AJ69" s="104"/>
       <c r="AK69" s="38"/>
       <c r="AL69" s="58"/>
       <c r="AM69" s="38"/>
@@ -24544,7 +24550,7 @@
         <v>253</v>
       </c>
       <c r="CL69" s="25" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="CM69" s="93"/>
     </row>
@@ -24584,7 +24590,7 @@
       <c r="AE70" s="40"/>
       <c r="AF70" s="40"/>
       <c r="AG70" s="40"/>
-      <c r="AH70" s="40"/>
+      <c r="AH70" s="98"/>
       <c r="AI70" s="38"/>
       <c r="AJ70" s="58"/>
       <c r="AK70" s="38"/>
@@ -24643,7 +24649,7 @@
         <v>254</v>
       </c>
       <c r="CL70" s="25" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="CM70" s="93"/>
     </row>
@@ -24683,7 +24689,7 @@
       <c r="AE71" s="40"/>
       <c r="AF71" s="40"/>
       <c r="AG71" s="40"/>
-      <c r="AH71" s="42"/>
+      <c r="AH71" s="40"/>
       <c r="AI71" s="38"/>
       <c r="AJ71" s="58"/>
       <c r="AK71" s="38"/>
@@ -24695,7 +24701,7 @@
       <c r="AQ71" s="56"/>
       <c r="AR71" s="58"/>
       <c r="AS71" s="40"/>
-      <c r="AT71" s="42"/>
+      <c r="AT71" s="40"/>
       <c r="AU71" s="40"/>
       <c r="AV71" s="38"/>
       <c r="AW71" s="58"/>
@@ -24728,7 +24734,7 @@
       <c r="BX71" s="58"/>
       <c r="BY71" s="38"/>
       <c r="BZ71" s="58"/>
-      <c r="CA71" s="61"/>
+      <c r="CA71" s="38"/>
       <c r="CB71" s="58"/>
       <c r="CC71" s="38"/>
       <c r="CD71" s="58"/>
@@ -24742,7 +24748,7 @@
         <v>255</v>
       </c>
       <c r="CL71" s="25" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="CM71" s="93"/>
     </row>
@@ -24782,7 +24788,7 @@
       <c r="AE72" s="40"/>
       <c r="AF72" s="40"/>
       <c r="AG72" s="40"/>
-      <c r="AH72" s="40"/>
+      <c r="AH72" s="42"/>
       <c r="AI72" s="38"/>
       <c r="AJ72" s="58"/>
       <c r="AK72" s="38"/>
@@ -24794,7 +24800,7 @@
       <c r="AQ72" s="56"/>
       <c r="AR72" s="58"/>
       <c r="AS72" s="40"/>
-      <c r="AT72" s="40"/>
+      <c r="AT72" s="42"/>
       <c r="AU72" s="40"/>
       <c r="AV72" s="38"/>
       <c r="AW72" s="58"/>
@@ -24827,7 +24833,7 @@
       <c r="BX72" s="58"/>
       <c r="BY72" s="38"/>
       <c r="BZ72" s="58"/>
-      <c r="CA72" s="38"/>
+      <c r="CA72" s="61"/>
       <c r="CB72" s="58"/>
       <c r="CC72" s="38"/>
       <c r="CD72" s="58"/>
@@ -24841,7 +24847,7 @@
         <v>256</v>
       </c>
       <c r="CL72" s="25" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="CM72" s="93"/>
     </row>
@@ -24884,7 +24890,7 @@
       <c r="AH73" s="40"/>
       <c r="AI73" s="38"/>
       <c r="AJ73" s="58"/>
-      <c r="AK73" s="61"/>
+      <c r="AK73" s="38"/>
       <c r="AL73" s="58"/>
       <c r="AM73" s="38"/>
       <c r="AN73" s="56"/>
@@ -24892,9 +24898,9 @@
       <c r="AP73" s="38"/>
       <c r="AQ73" s="56"/>
       <c r="AR73" s="58"/>
-      <c r="AS73" s="42"/>
-      <c r="AT73" s="42"/>
-      <c r="AU73" s="42"/>
+      <c r="AS73" s="40"/>
+      <c r="AT73" s="40"/>
+      <c r="AU73" s="40"/>
       <c r="AV73" s="38"/>
       <c r="AW73" s="58"/>
       <c r="AX73" s="40"/>
@@ -24922,11 +24928,11 @@
       <c r="BT73" s="40"/>
       <c r="BU73" s="40"/>
       <c r="BV73" s="40"/>
-      <c r="BW73" s="61"/>
+      <c r="BW73" s="38"/>
       <c r="BX73" s="58"/>
-      <c r="BY73" s="61"/>
+      <c r="BY73" s="38"/>
       <c r="BZ73" s="58"/>
-      <c r="CA73" s="61"/>
+      <c r="CA73" s="38"/>
       <c r="CB73" s="58"/>
       <c r="CC73" s="38"/>
       <c r="CD73" s="58"/>
@@ -24940,7 +24946,7 @@
         <v>257</v>
       </c>
       <c r="CL73" s="25" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="CM73" s="93"/>
     </row>
@@ -24991,8 +24997,8 @@
       <c r="AP74" s="38"/>
       <c r="AQ74" s="56"/>
       <c r="AR74" s="58"/>
-      <c r="AS74" s="40"/>
-      <c r="AT74" s="40"/>
+      <c r="AS74" s="42"/>
+      <c r="AT74" s="42"/>
       <c r="AU74" s="42"/>
       <c r="AV74" s="38"/>
       <c r="AW74" s="58"/>
@@ -25019,13 +25025,13 @@
       <c r="BR74" s="40"/>
       <c r="BS74" s="40"/>
       <c r="BT74" s="40"/>
-      <c r="BU74" s="42"/>
+      <c r="BU74" s="40"/>
       <c r="BV74" s="40"/>
       <c r="BW74" s="61"/>
       <c r="BX74" s="58"/>
       <c r="BY74" s="61"/>
       <c r="BZ74" s="58"/>
-      <c r="CA74" s="38"/>
+      <c r="CA74" s="61"/>
       <c r="CB74" s="58"/>
       <c r="CC74" s="38"/>
       <c r="CD74" s="58"/>
@@ -25039,7 +25045,7 @@
         <v>258</v>
       </c>
       <c r="CL74" s="25" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="CM74" s="93"/>
     </row>
@@ -25118,7 +25124,7 @@
       <c r="BR75" s="40"/>
       <c r="BS75" s="40"/>
       <c r="BT75" s="40"/>
-      <c r="BU75" s="40"/>
+      <c r="BU75" s="42"/>
       <c r="BV75" s="40"/>
       <c r="BW75" s="61"/>
       <c r="BX75" s="58"/>
@@ -25138,230 +25144,228 @@
         <v>259</v>
       </c>
       <c r="CL75" s="25" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="CM75" s="93"/>
     </row>
-    <row r="76" spans="1:91" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A76" s="93"/>
-      <c r="B76" s="31"/>
-      <c r="C76" s="92" t="s">
+      <c r="B76" s="30"/>
+      <c r="C76" s="25" t="s">
         <v>260</v>
       </c>
-      <c r="D76" s="41"/>
-      <c r="E76" s="41"/>
-      <c r="F76" s="41"/>
-      <c r="G76" s="41"/>
-      <c r="H76" s="41"/>
-      <c r="I76" s="41"/>
-      <c r="J76" s="41"/>
-      <c r="K76" s="41"/>
-      <c r="L76" s="41"/>
-      <c r="M76" s="41"/>
-      <c r="N76" s="59"/>
-      <c r="O76" s="60"/>
-      <c r="P76" s="59"/>
-      <c r="Q76" s="60"/>
-      <c r="R76" s="59"/>
-      <c r="S76" s="60"/>
-      <c r="T76" s="59"/>
-      <c r="U76" s="60"/>
-      <c r="V76" s="41"/>
-      <c r="W76" s="41"/>
-      <c r="X76" s="41"/>
-      <c r="Y76" s="59"/>
-      <c r="Z76" s="60"/>
-      <c r="AA76" s="59"/>
-      <c r="AB76" s="60"/>
-      <c r="AC76" s="59"/>
-      <c r="AD76" s="60"/>
-      <c r="AE76" s="41"/>
-      <c r="AF76" s="41"/>
-      <c r="AG76" s="41"/>
-      <c r="AH76" s="102"/>
-      <c r="AI76" s="59"/>
-      <c r="AJ76" s="105"/>
-      <c r="AK76" s="59"/>
-      <c r="AL76" s="60"/>
-      <c r="AM76" s="59"/>
-      <c r="AN76" s="74"/>
-      <c r="AO76" s="60"/>
-      <c r="AP76" s="59"/>
-      <c r="AQ76" s="74"/>
-      <c r="AR76" s="60"/>
-      <c r="AS76" s="41"/>
-      <c r="AT76" s="41"/>
-      <c r="AU76" s="41"/>
-      <c r="AV76" s="59"/>
-      <c r="AW76" s="60"/>
-      <c r="AX76" s="41"/>
-      <c r="AY76" s="41"/>
-      <c r="AZ76" s="59"/>
-      <c r="BA76" s="60"/>
-      <c r="BB76" s="59"/>
-      <c r="BC76" s="74"/>
-      <c r="BD76" s="60"/>
-      <c r="BE76" s="59"/>
-      <c r="BF76" s="74"/>
-      <c r="BG76" s="60"/>
-      <c r="BH76" s="59"/>
-      <c r="BI76" s="60"/>
-      <c r="BJ76" s="41"/>
-      <c r="BK76" s="59"/>
-      <c r="BL76" s="74"/>
-      <c r="BM76" s="60"/>
-      <c r="BN76" s="59"/>
-      <c r="BO76" s="74"/>
-      <c r="BP76" s="74"/>
-      <c r="BQ76" s="60"/>
-      <c r="BR76" s="41"/>
-      <c r="BS76" s="41"/>
-      <c r="BT76" s="41"/>
-      <c r="BU76" s="41"/>
-      <c r="BV76" s="41"/>
-      <c r="BW76" s="59"/>
-      <c r="BX76" s="60"/>
-      <c r="BY76" s="59"/>
-      <c r="BZ76" s="60"/>
-      <c r="CA76" s="59"/>
-      <c r="CB76" s="60"/>
-      <c r="CC76" s="59"/>
-      <c r="CD76" s="60"/>
-      <c r="CE76" s="41"/>
-      <c r="CF76" s="41"/>
-      <c r="CG76" s="41"/>
-      <c r="CH76" s="41"/>
-      <c r="CI76" s="41"/>
-      <c r="CJ76" s="41"/>
-      <c r="CK76" s="91" t="s">
+      <c r="D76" s="40"/>
+      <c r="E76" s="40"/>
+      <c r="F76" s="40"/>
+      <c r="G76" s="40"/>
+      <c r="H76" s="40"/>
+      <c r="I76" s="40"/>
+      <c r="J76" s="40"/>
+      <c r="K76" s="40"/>
+      <c r="L76" s="40"/>
+      <c r="M76" s="40"/>
+      <c r="N76" s="38"/>
+      <c r="O76" s="58"/>
+      <c r="P76" s="38"/>
+      <c r="Q76" s="58"/>
+      <c r="R76" s="38"/>
+      <c r="S76" s="58"/>
+      <c r="T76" s="38"/>
+      <c r="U76" s="58"/>
+      <c r="V76" s="40"/>
+      <c r="W76" s="40"/>
+      <c r="X76" s="40"/>
+      <c r="Y76" s="38"/>
+      <c r="Z76" s="58"/>
+      <c r="AA76" s="38"/>
+      <c r="AB76" s="58"/>
+      <c r="AC76" s="38"/>
+      <c r="AD76" s="58"/>
+      <c r="AE76" s="40"/>
+      <c r="AF76" s="40"/>
+      <c r="AG76" s="40"/>
+      <c r="AH76" s="40"/>
+      <c r="AI76" s="38"/>
+      <c r="AJ76" s="58"/>
+      <c r="AK76" s="61"/>
+      <c r="AL76" s="58"/>
+      <c r="AM76" s="38"/>
+      <c r="AN76" s="56"/>
+      <c r="AO76" s="58"/>
+      <c r="AP76" s="38"/>
+      <c r="AQ76" s="56"/>
+      <c r="AR76" s="58"/>
+      <c r="AS76" s="40"/>
+      <c r="AT76" s="40"/>
+      <c r="AU76" s="42"/>
+      <c r="AV76" s="38"/>
+      <c r="AW76" s="58"/>
+      <c r="AX76" s="40"/>
+      <c r="AY76" s="40"/>
+      <c r="AZ76" s="38"/>
+      <c r="BA76" s="58"/>
+      <c r="BB76" s="38"/>
+      <c r="BC76" s="56"/>
+      <c r="BD76" s="58"/>
+      <c r="BE76" s="38"/>
+      <c r="BF76" s="56"/>
+      <c r="BG76" s="58"/>
+      <c r="BH76" s="38"/>
+      <c r="BI76" s="58"/>
+      <c r="BJ76" s="40"/>
+      <c r="BK76" s="38"/>
+      <c r="BL76" s="56"/>
+      <c r="BM76" s="58"/>
+      <c r="BN76" s="38"/>
+      <c r="BO76" s="56"/>
+      <c r="BP76" s="56"/>
+      <c r="BQ76" s="58"/>
+      <c r="BR76" s="40"/>
+      <c r="BS76" s="40"/>
+      <c r="BT76" s="40"/>
+      <c r="BU76" s="40"/>
+      <c r="BV76" s="40"/>
+      <c r="BW76" s="61"/>
+      <c r="BX76" s="58"/>
+      <c r="BY76" s="61"/>
+      <c r="BZ76" s="58"/>
+      <c r="CA76" s="38"/>
+      <c r="CB76" s="58"/>
+      <c r="CC76" s="38"/>
+      <c r="CD76" s="58"/>
+      <c r="CE76" s="40"/>
+      <c r="CF76" s="40"/>
+      <c r="CG76" s="40"/>
+      <c r="CH76" s="40"/>
+      <c r="CI76" s="40"/>
+      <c r="CJ76" s="40"/>
+      <c r="CK76" s="90" t="s">
         <v>260</v>
       </c>
-      <c r="CL76" s="92" t="s">
-        <v>333</v>
+      <c r="CL76" s="25" t="s">
+        <v>334</v>
       </c>
       <c r="CM76" s="93"/>
     </row>
-    <row r="77" spans="1:91" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:91" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A77" s="93"/>
-      <c r="B77" s="93"/>
-      <c r="C77" s="93"/>
-      <c r="D77" s="93"/>
-      <c r="E77" s="93"/>
-      <c r="F77" s="93"/>
-      <c r="G77" s="93"/>
-      <c r="H77" s="93"/>
-      <c r="I77" s="93"/>
-      <c r="J77" s="93"/>
-      <c r="K77" s="93"/>
-      <c r="L77" s="93"/>
-      <c r="M77" s="93"/>
-      <c r="N77" s="93"/>
-      <c r="O77" s="93"/>
-      <c r="P77" s="93"/>
-      <c r="Q77" s="93"/>
-      <c r="R77" s="93"/>
-      <c r="S77" s="93"/>
-      <c r="T77" s="93"/>
-      <c r="U77" s="93"/>
-      <c r="V77" s="93"/>
-      <c r="W77" s="93"/>
-      <c r="X77" s="93"/>
-      <c r="Y77" s="93"/>
-      <c r="Z77" s="93"/>
-      <c r="AA77" s="93"/>
-      <c r="AB77" s="93"/>
-      <c r="AC77" s="93"/>
-      <c r="AD77" s="93"/>
-      <c r="AE77" s="93"/>
-      <c r="AF77" s="93"/>
-      <c r="AG77" s="93"/>
-      <c r="AH77" s="93"/>
-      <c r="AI77" s="93"/>
-      <c r="AJ77" s="93"/>
-      <c r="AK77" s="93"/>
-      <c r="AL77" s="93"/>
-      <c r="AM77" s="93"/>
-      <c r="AN77" s="93"/>
-      <c r="AO77" s="93"/>
-      <c r="AP77" s="93"/>
-      <c r="AQ77" s="93"/>
-      <c r="AR77" s="93"/>
-      <c r="AS77" s="93"/>
-      <c r="AT77" s="93"/>
-      <c r="AU77" s="93"/>
-      <c r="AV77" s="93"/>
-      <c r="AW77" s="93"/>
-      <c r="AX77" s="93"/>
-      <c r="AY77" s="93"/>
-      <c r="AZ77" s="93"/>
-      <c r="BA77" s="93"/>
-      <c r="BB77" s="93"/>
-      <c r="BC77" s="93"/>
-      <c r="BD77" s="93"/>
-      <c r="BE77" s="93"/>
-      <c r="BF77" s="93"/>
-      <c r="BG77" s="93"/>
-      <c r="BH77" s="93"/>
-      <c r="BI77" s="93"/>
-      <c r="BJ77" s="93"/>
-      <c r="BK77" s="93"/>
-      <c r="BL77" s="93"/>
-      <c r="BM77" s="93"/>
-      <c r="BN77" s="93"/>
-      <c r="BO77" s="93"/>
-      <c r="BP77" s="93"/>
-      <c r="BQ77" s="93"/>
-      <c r="BR77" s="93"/>
-      <c r="BS77" s="93"/>
-      <c r="BT77" s="93"/>
-      <c r="BU77" s="93"/>
-      <c r="BV77" s="93"/>
-      <c r="BW77" s="93"/>
-      <c r="BX77" s="93"/>
-      <c r="BY77" s="93"/>
-      <c r="BZ77" s="93"/>
-      <c r="CA77" s="93"/>
-      <c r="CB77" s="93"/>
-      <c r="CC77" s="93"/>
-      <c r="CD77" s="93"/>
-      <c r="CE77" s="93"/>
-      <c r="CF77" s="93"/>
-      <c r="CG77" s="93"/>
-      <c r="CH77" s="93"/>
-      <c r="CI77" s="93"/>
-      <c r="CJ77" s="93"/>
-      <c r="CK77" s="93"/>
-      <c r="CL77" s="93"/>
+      <c r="B77" s="31"/>
+      <c r="C77" s="92" t="s">
+        <v>261</v>
+      </c>
+      <c r="D77" s="41"/>
+      <c r="E77" s="41"/>
+      <c r="F77" s="41"/>
+      <c r="G77" s="41"/>
+      <c r="H77" s="41"/>
+      <c r="I77" s="41"/>
+      <c r="J77" s="41"/>
+      <c r="K77" s="41"/>
+      <c r="L77" s="41"/>
+      <c r="M77" s="41"/>
+      <c r="N77" s="59"/>
+      <c r="O77" s="60"/>
+      <c r="P77" s="59"/>
+      <c r="Q77" s="60"/>
+      <c r="R77" s="59"/>
+      <c r="S77" s="60"/>
+      <c r="T77" s="59"/>
+      <c r="U77" s="60"/>
+      <c r="V77" s="41"/>
+      <c r="W77" s="41"/>
+      <c r="X77" s="41"/>
+      <c r="Y77" s="59"/>
+      <c r="Z77" s="60"/>
+      <c r="AA77" s="59"/>
+      <c r="AB77" s="60"/>
+      <c r="AC77" s="59"/>
+      <c r="AD77" s="60"/>
+      <c r="AE77" s="41"/>
+      <c r="AF77" s="41"/>
+      <c r="AG77" s="41"/>
+      <c r="AH77" s="102"/>
+      <c r="AI77" s="59"/>
+      <c r="AJ77" s="105"/>
+      <c r="AK77" s="59"/>
+      <c r="AL77" s="60"/>
+      <c r="AM77" s="59"/>
+      <c r="AN77" s="74"/>
+      <c r="AO77" s="60"/>
+      <c r="AP77" s="59"/>
+      <c r="AQ77" s="74"/>
+      <c r="AR77" s="60"/>
+      <c r="AS77" s="41"/>
+      <c r="AT77" s="41"/>
+      <c r="AU77" s="41"/>
+      <c r="AV77" s="59"/>
+      <c r="AW77" s="60"/>
+      <c r="AX77" s="41"/>
+      <c r="AY77" s="41"/>
+      <c r="AZ77" s="59"/>
+      <c r="BA77" s="60"/>
+      <c r="BB77" s="59"/>
+      <c r="BC77" s="74"/>
+      <c r="BD77" s="60"/>
+      <c r="BE77" s="59"/>
+      <c r="BF77" s="74"/>
+      <c r="BG77" s="60"/>
+      <c r="BH77" s="59"/>
+      <c r="BI77" s="60"/>
+      <c r="BJ77" s="41"/>
+      <c r="BK77" s="59"/>
+      <c r="BL77" s="74"/>
+      <c r="BM77" s="60"/>
+      <c r="BN77" s="59"/>
+      <c r="BO77" s="74"/>
+      <c r="BP77" s="74"/>
+      <c r="BQ77" s="60"/>
+      <c r="BR77" s="41"/>
+      <c r="BS77" s="41"/>
+      <c r="BT77" s="41"/>
+      <c r="BU77" s="41"/>
+      <c r="BV77" s="41"/>
+      <c r="BW77" s="59"/>
+      <c r="BX77" s="60"/>
+      <c r="BY77" s="59"/>
+      <c r="BZ77" s="60"/>
+      <c r="CA77" s="59"/>
+      <c r="CB77" s="60"/>
+      <c r="CC77" s="59"/>
+      <c r="CD77" s="60"/>
+      <c r="CE77" s="41"/>
+      <c r="CF77" s="41"/>
+      <c r="CG77" s="41"/>
+      <c r="CH77" s="41"/>
+      <c r="CI77" s="41"/>
+      <c r="CJ77" s="41"/>
+      <c r="CK77" s="91" t="s">
+        <v>261</v>
+      </c>
+      <c r="CL77" s="92" t="s">
+        <v>335</v>
+      </c>
       <c r="CM77" s="93"/>
     </row>
-    <row r="78" spans="1:91" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:91" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="93"/>
       <c r="B78" s="93"/>
       <c r="C78" s="93"/>
       <c r="D78" s="93"/>
-      <c r="E78" s="75"/>
-      <c r="F78" s="94" t="s">
-        <v>179</v>
-      </c>
+      <c r="E78" s="93"/>
+      <c r="F78" s="93"/>
       <c r="G78" s="93"/>
       <c r="H78" s="93"/>
       <c r="I78" s="93"/>
-      <c r="J78" s="82">
-        <v>3</v>
-      </c>
-      <c r="K78" s="94" t="s">
-        <v>180</v>
-      </c>
+      <c r="J78" s="93"/>
+      <c r="K78" s="93"/>
       <c r="L78" s="93"/>
       <c r="M78" s="93"/>
       <c r="N78" s="93"/>
       <c r="O78" s="93"/>
       <c r="P78" s="93"/>
       <c r="Q78" s="93"/>
-      <c r="R78" s="96"/>
-      <c r="S78" s="94" t="s">
-        <v>181</v>
-      </c>
+      <c r="R78" s="93"/>
+      <c r="S78" s="93"/>
       <c r="T78" s="93"/>
       <c r="U78" s="93"/>
       <c r="V78" s="93"/>
@@ -25440,21 +25444,29 @@
       <c r="B79" s="93"/>
       <c r="C79" s="93"/>
       <c r="D79" s="93"/>
-      <c r="E79" s="93"/>
-      <c r="F79" s="93"/>
+      <c r="E79" s="75"/>
+      <c r="F79" s="94" t="s">
+        <v>179</v>
+      </c>
       <c r="G79" s="93"/>
       <c r="H79" s="93"/>
       <c r="I79" s="93"/>
-      <c r="J79" s="93"/>
-      <c r="K79" s="93"/>
+      <c r="J79" s="82">
+        <v>3</v>
+      </c>
+      <c r="K79" s="94" t="s">
+        <v>180</v>
+      </c>
       <c r="L79" s="93"/>
       <c r="M79" s="93"/>
       <c r="N79" s="93"/>
       <c r="O79" s="93"/>
       <c r="P79" s="93"/>
       <c r="Q79" s="93"/>
-      <c r="R79" s="93"/>
-      <c r="S79" s="93"/>
+      <c r="R79" s="96"/>
+      <c r="S79" s="94" t="s">
+        <v>181</v>
+      </c>
       <c r="T79" s="93"/>
       <c r="U79" s="93"/>
       <c r="V79" s="93"/>
@@ -29899,6 +29911,99 @@
       <c r="CL126" s="93"/>
       <c r="CM126" s="93"/>
     </row>
+    <row r="127" spans="1:91" x14ac:dyDescent="0.2">
+      <c r="A127" s="93"/>
+      <c r="B127" s="93"/>
+      <c r="C127" s="93"/>
+      <c r="D127" s="93"/>
+      <c r="E127" s="93"/>
+      <c r="F127" s="93"/>
+      <c r="G127" s="93"/>
+      <c r="H127" s="93"/>
+      <c r="I127" s="93"/>
+      <c r="J127" s="93"/>
+      <c r="K127" s="93"/>
+      <c r="L127" s="93"/>
+      <c r="M127" s="93"/>
+      <c r="N127" s="93"/>
+      <c r="O127" s="93"/>
+      <c r="P127" s="93"/>
+      <c r="Q127" s="93"/>
+      <c r="R127" s="93"/>
+      <c r="S127" s="93"/>
+      <c r="T127" s="93"/>
+      <c r="U127" s="93"/>
+      <c r="V127" s="93"/>
+      <c r="W127" s="93"/>
+      <c r="X127" s="93"/>
+      <c r="Y127" s="93"/>
+      <c r="Z127" s="93"/>
+      <c r="AA127" s="93"/>
+      <c r="AB127" s="93"/>
+      <c r="AC127" s="93"/>
+      <c r="AD127" s="93"/>
+      <c r="AE127" s="93"/>
+      <c r="AF127" s="93"/>
+      <c r="AG127" s="93"/>
+      <c r="AH127" s="93"/>
+      <c r="AI127" s="93"/>
+      <c r="AJ127" s="93"/>
+      <c r="AK127" s="93"/>
+      <c r="AL127" s="93"/>
+      <c r="AM127" s="93"/>
+      <c r="AN127" s="93"/>
+      <c r="AO127" s="93"/>
+      <c r="AP127" s="93"/>
+      <c r="AQ127" s="93"/>
+      <c r="AR127" s="93"/>
+      <c r="AS127" s="93"/>
+      <c r="AT127" s="93"/>
+      <c r="AU127" s="93"/>
+      <c r="AV127" s="93"/>
+      <c r="AW127" s="93"/>
+      <c r="AX127" s="93"/>
+      <c r="AY127" s="93"/>
+      <c r="AZ127" s="93"/>
+      <c r="BA127" s="93"/>
+      <c r="BB127" s="93"/>
+      <c r="BC127" s="93"/>
+      <c r="BD127" s="93"/>
+      <c r="BE127" s="93"/>
+      <c r="BF127" s="93"/>
+      <c r="BG127" s="93"/>
+      <c r="BH127" s="93"/>
+      <c r="BI127" s="93"/>
+      <c r="BJ127" s="93"/>
+      <c r="BK127" s="93"/>
+      <c r="BL127" s="93"/>
+      <c r="BM127" s="93"/>
+      <c r="BN127" s="93"/>
+      <c r="BO127" s="93"/>
+      <c r="BP127" s="93"/>
+      <c r="BQ127" s="93"/>
+      <c r="BR127" s="93"/>
+      <c r="BS127" s="93"/>
+      <c r="BT127" s="93"/>
+      <c r="BU127" s="93"/>
+      <c r="BV127" s="93"/>
+      <c r="BW127" s="93"/>
+      <c r="BX127" s="93"/>
+      <c r="BY127" s="93"/>
+      <c r="BZ127" s="93"/>
+      <c r="CA127" s="93"/>
+      <c r="CB127" s="93"/>
+      <c r="CC127" s="93"/>
+      <c r="CD127" s="93"/>
+      <c r="CE127" s="93"/>
+      <c r="CF127" s="93"/>
+      <c r="CG127" s="93"/>
+      <c r="CH127" s="93"/>
+      <c r="CI127" s="93"/>
+      <c r="CJ127" s="93"/>
+      <c r="CK127" s="93"/>
+      <c r="CL127" s="93"/>
+      <c r="CM127" s="93"/>
+    </row>
   </sheetData>
   <mergeCells count="22">
     <mergeCell ref="BW2:BX2"/>
@@ -29948,7 +30053,7 @@
     <row r="1" spans="1:21" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="93"/>
       <c r="B1" s="95" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="C1" s="93"/>
       <c r="D1" s="93"/>
@@ -30039,7 +30144,7 @@
       <c r="K3" s="118"/>
       <c r="L3" s="118"/>
       <c r="M3" s="119" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="N3" s="118"/>
       <c r="O3" s="118"/>
@@ -30053,10 +30158,10 @@
     <row r="4" spans="1:21" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="93"/>
       <c r="B4" s="2" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="C4" s="43" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="D4" s="45">
         <v>1</v>
@@ -30107,17 +30212,17 @@
         <v>1</v>
       </c>
       <c r="T4" s="120" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="U4" s="93"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="93"/>
       <c r="B5" s="15" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="C5" s="84" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="D5" s="99">
         <v>700</v>
@@ -30168,7 +30273,7 @@
         <v>36</v>
       </c>
       <c r="T5" s="121" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="U5" s="93"/>
     </row>
@@ -30176,7 +30281,7 @@
       <c r="A6" s="93"/>
       <c r="B6" s="109"/>
       <c r="C6" s="86" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="D6" s="97">
         <v>950</v>
@@ -30227,7 +30332,7 @@
         <v>36</v>
       </c>
       <c r="T6" s="122" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="U6" s="93"/>
     </row>
@@ -30235,7 +30340,7 @@
       <c r="A7" s="93"/>
       <c r="B7" s="109"/>
       <c r="C7" s="86" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="D7" s="97">
         <v>2150</v>
@@ -30286,7 +30391,7 @@
         <v>2150</v>
       </c>
       <c r="T7" s="122" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="U7" s="93"/>
     </row>
@@ -30294,7 +30399,7 @@
       <c r="A8" s="93"/>
       <c r="B8" s="110"/>
       <c r="C8" s="88" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="D8" s="113">
         <v>2300</v>
@@ -30345,17 +30450,17 @@
         <v>2250</v>
       </c>
       <c r="T8" s="123" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="U8" s="93"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="93"/>
       <c r="B9" s="29" t="s">
+        <v>344</v>
+      </c>
+      <c r="C9" s="89" t="s">
         <v>342</v>
-      </c>
-      <c r="C9" s="89" t="s">
-        <v>340</v>
       </c>
       <c r="D9" s="114">
         <v>-27</v>
@@ -30406,7 +30511,7 @@
         <v>-25</v>
       </c>
       <c r="T9" s="124" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="U9" s="93"/>
     </row>
@@ -30414,7 +30519,7 @@
       <c r="A10" s="93"/>
       <c r="B10" s="111"/>
       <c r="C10" s="92" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="D10" s="115">
         <v>20</v>
@@ -30465,17 +30570,17 @@
         <v>20</v>
       </c>
       <c r="T10" s="125" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="U10" s="93"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="93"/>
       <c r="B11" s="15" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="C11" s="84" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="D11" s="99">
         <v>8.7999999999999995E-2</v>
@@ -30526,7 +30631,7 @@
         <v>0.08</v>
       </c>
       <c r="T11" s="121" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="U11" s="93"/>
     </row>
@@ -30534,7 +30639,7 @@
       <c r="A12" s="93"/>
       <c r="B12" s="109"/>
       <c r="C12" s="86" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="D12" s="97">
         <v>8.7999999999999995E-2</v>
@@ -30585,7 +30690,7 @@
         <v>0.08</v>
       </c>
       <c r="T12" s="122" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="U12" s="93"/>
     </row>
@@ -30593,7 +30698,7 @@
       <c r="A13" s="93"/>
       <c r="B13" s="109"/>
       <c r="C13" s="86" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="D13" s="97">
         <v>45</v>
@@ -30644,7 +30749,7 @@
         <v>70</v>
       </c>
       <c r="T13" s="122" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="U13" s="93"/>
     </row>
@@ -30652,7 +30757,7 @@
       <c r="A14" s="93"/>
       <c r="B14" s="110"/>
       <c r="C14" s="88" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="D14" s="113">
         <v>45</v>
@@ -30703,17 +30808,17 @@
         <v>70</v>
       </c>
       <c r="T14" s="123" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="U14" s="93"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="93"/>
       <c r="B15" s="29" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="C15" s="89" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="D15" s="114">
         <v>8.7999999999999995E-2</v>
@@ -30764,7 +30869,7 @@
         <v>0.08</v>
       </c>
       <c r="T15" s="124" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="U15" s="93"/>
     </row>
@@ -30772,7 +30877,7 @@
       <c r="A16" s="93"/>
       <c r="B16" s="112"/>
       <c r="C16" s="25" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="D16" s="116">
         <v>8.7999999999999995E-2</v>
@@ -30823,7 +30928,7 @@
         <v>0.08</v>
       </c>
       <c r="T16" s="126" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="U16" s="93"/>
     </row>
@@ -30831,7 +30936,7 @@
       <c r="A17" s="93"/>
       <c r="B17" s="112"/>
       <c r="C17" s="25" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="D17" s="116">
         <v>45</v>
@@ -30882,7 +30987,7 @@
         <v>70</v>
       </c>
       <c r="T17" s="126" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="U17" s="93"/>
     </row>
@@ -30890,7 +30995,7 @@
       <c r="A18" s="93"/>
       <c r="B18" s="111"/>
       <c r="C18" s="92" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="D18" s="115">
         <v>45</v>
@@ -30941,7 +31046,7 @@
         <v>70</v>
       </c>
       <c r="T18" s="125" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="U18" s="93"/>
     </row>
@@ -32120,7 +32225,7 @@
     <row r="1" spans="1:19" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="93"/>
       <c r="B1" s="95" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="C1" s="93"/>
       <c r="D1" s="93"/>
@@ -32213,10 +32318,10 @@
     <row r="4" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="93"/>
       <c r="B4" s="2" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="C4" s="43" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="D4" s="45">
         <v>1</v>
@@ -32261,17 +32366,17 @@
         <v>1</v>
       </c>
       <c r="R4" s="120" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="S4" s="93"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="93"/>
       <c r="B5" s="15" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="C5" s="84" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="D5" s="99">
         <v>950</v>
@@ -32316,7 +32421,7 @@
         <v>42</v>
       </c>
       <c r="R5" s="121" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="S5" s="93"/>
     </row>
@@ -32324,7 +32429,7 @@
       <c r="A6" s="93"/>
       <c r="B6" s="109"/>
       <c r="C6" s="86" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="D6" s="97">
         <v>950</v>
@@ -32369,7 +32474,7 @@
         <v>42</v>
       </c>
       <c r="R6" s="122" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="S6" s="93"/>
     </row>
@@ -32377,7 +32482,7 @@
       <c r="A7" s="93"/>
       <c r="B7" s="109"/>
       <c r="C7" s="86" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="D7" s="97">
         <v>2150</v>
@@ -32422,7 +32527,7 @@
         <v>1002</v>
       </c>
       <c r="R7" s="122" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="S7" s="93"/>
     </row>
@@ -32430,7 +32535,7 @@
       <c r="A8" s="93"/>
       <c r="B8" s="110"/>
       <c r="C8" s="88" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="D8" s="113">
         <v>2150</v>
@@ -32475,7 +32580,7 @@
         <v>1002</v>
       </c>
       <c r="R8" s="123" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="S8" s="93"/>
     </row>

</xml_diff>